<commit_message>
New version. TPS and CSP issues are resolved.
</commit_message>
<xml_diff>
--- a/Book chapter Studies/Data to optimization/KPIs-7-03-2025.xlsx
+++ b/Book chapter Studies/Data to optimization/KPIs-7-03-2025.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\szata\Codes\StoriesTeams\Pipeline-dispatcher\Book chapter Studies\Data to optimization\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6050EAF4-DC63-4601-B6BD-65DBCE463362}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00AF16F7-6F06-47A1-8DE7-CB2D71E8D80A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -78,7 +78,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="86">
   <si>
     <t>HP</t>
   </si>
@@ -299,9 +299,6 @@
     <t>mismatch th</t>
   </si>
   <si>
-    <t>Total el loss</t>
-  </si>
-  <si>
     <t>Total Generation</t>
   </si>
   <si>
@@ -335,17 +332,17 @@
     <t>High price</t>
   </si>
   <si>
-    <t>Total el consumption</t>
-  </si>
-  <si>
-    <t>Total th consumption</t>
+    <t>import in LPT</t>
+  </si>
+  <si>
+    <t>Export in HPT</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -391,12 +388,6 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Aptos Narrow"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -519,7 +510,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -553,14 +544,12 @@
     <xf numFmtId="0" fontId="5" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -857,7 +846,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AC35"/>
   <sheetViews>
-    <sheetView topLeftCell="N1" workbookViewId="0">
+    <sheetView topLeftCell="E1" workbookViewId="0">
       <selection activeCell="L13" sqref="J1:L13"/>
     </sheetView>
   </sheetViews>
@@ -2549,8 +2538,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6764646B-423B-4E75-A577-25C6655501A4}">
   <dimension ref="A1:AH26"/>
   <sheetViews>
-    <sheetView topLeftCell="U1" workbookViewId="0">
-      <selection activeCell="AH23" sqref="AH23"/>
+    <sheetView topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="AC14" sqref="A1:AH26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2563,16 +2552,16 @@
     <col min="27" max="27" width="10.6640625" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="10.77734375" bestFit="1" customWidth="1"/>
     <col min="29" max="30" width="12.88671875" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="17.6640625" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="17.77734375" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:34" x14ac:dyDescent="0.3">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="31" t="s">
+        <v>79</v>
+      </c>
+      <c r="B1" s="32" t="s">
         <v>80</v>
-      </c>
-      <c r="B1" s="33" t="s">
-        <v>81</v>
       </c>
       <c r="C1" s="26" t="s">
         <v>45</v>
@@ -2659,91 +2648,91 @@
         <v>70</v>
       </c>
       <c r="AE1" s="29" t="s">
+        <v>82</v>
+      </c>
+      <c r="AF1" s="29" t="s">
         <v>83</v>
       </c>
-      <c r="AF1" s="29" t="s">
+      <c r="AG1" s="29" t="s">
         <v>84</v>
       </c>
-      <c r="AG1" s="29" t="s">
+      <c r="AH1" s="29" t="s">
         <v>85</v>
       </c>
-      <c r="AH1" s="29" t="s">
-        <v>86</v>
-      </c>
     </row>
     <row r="2" spans="1:34" x14ac:dyDescent="0.3">
-      <c r="A2" s="32">
+      <c r="A2" s="31">
         <v>0.26038899999999998</v>
       </c>
       <c r="B2" s="26">
         <v>0</v>
       </c>
-      <c r="C2" s="26">
-        <v>0</v>
-      </c>
-      <c r="D2" s="26">
-        <v>0</v>
-      </c>
-      <c r="E2" s="26">
-        <v>-391736</v>
-      </c>
-      <c r="F2" s="26">
-        <v>0</v>
-      </c>
-      <c r="G2" s="26">
-        <v>0</v>
-      </c>
-      <c r="H2" s="26">
-        <v>0</v>
-      </c>
-      <c r="I2" s="26">
-        <v>0</v>
-      </c>
-      <c r="J2" s="26">
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>-391735.72530890797</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+      <c r="J2">
         <v>168750</v>
       </c>
-      <c r="K2" s="26">
-        <v>0</v>
-      </c>
-      <c r="L2" s="26">
-        <v>0</v>
-      </c>
-      <c r="M2" s="26">
-        <v>0</v>
-      </c>
-      <c r="N2" s="26">
-        <v>0</v>
-      </c>
-      <c r="O2" s="26">
-        <v>0</v>
-      </c>
-      <c r="P2" s="26">
+      <c r="K2">
+        <v>0</v>
+      </c>
+      <c r="L2">
+        <v>0</v>
+      </c>
+      <c r="M2">
+        <v>0</v>
+      </c>
+      <c r="N2">
+        <v>0</v>
+      </c>
+      <c r="O2">
+        <v>-62750</v>
+      </c>
+      <c r="P2">
         <v>0.5</v>
       </c>
-      <c r="Q2" s="26">
+      <c r="Q2">
         <v>0.5</v>
       </c>
-      <c r="R2" s="26">
+      <c r="R2">
         <v>0.5</v>
       </c>
-      <c r="S2" s="26">
+      <c r="S2">
         <v>0.5</v>
       </c>
-      <c r="T2" s="26">
-        <v>-222986</v>
-      </c>
-      <c r="U2" s="26">
-        <v>0</v>
-      </c>
-      <c r="V2" s="26">
-        <v>0.25468499999999999</v>
-      </c>
-      <c r="W2" s="26">
+      <c r="T2">
+        <v>-222985.725308908</v>
+      </c>
+      <c r="U2">
+        <v>-62750</v>
+      </c>
+      <c r="V2">
+        <v>0.254685102</v>
+      </c>
+      <c r="W2">
         <v>0.19520999999999999</v>
       </c>
       <c r="X2" s="28">
         <f>IF(T2&lt;0,T2,0)</f>
-        <v>-222986</v>
+        <v>-222985.725308908</v>
       </c>
       <c r="Y2" s="28">
         <f>IF(T2&gt;0,T2,0)</f>
@@ -2751,7 +2740,7 @@
       </c>
       <c r="Z2" s="28">
         <f>IF(U2&lt;0,U2,0)</f>
-        <v>0</v>
+        <v>-62750</v>
       </c>
       <c r="AA2" s="28">
         <f>IF(U2&gt;0,U2,0)</f>
@@ -2767,7 +2756,7 @@
       </c>
       <c r="AD2" s="30">
         <f>SUM(C2,D2,E2,F2,G2,H2,I2,J2,N2,O2,-X2,-Y2,-Z2,-AA2)</f>
-        <v>0</v>
+        <v>2.9103830456733704E-11</v>
       </c>
       <c r="AE2" s="30">
         <f>IF('Day1'!A2&lt;KPI!$B$15,1,0)</f>
@@ -2778,87 +2767,87 @@
         <v>0</v>
       </c>
       <c r="AG2" s="30">
-        <f>E2</f>
-        <v>-391736</v>
+        <f>X2*AE2</f>
+        <v>-222985.725308908</v>
       </c>
       <c r="AH2" s="30">
-        <f>O2</f>
+        <f>Y2*AF2</f>
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:34" x14ac:dyDescent="0.3">
-      <c r="A3" s="32">
+      <c r="A3" s="31">
         <v>0.25714300000000001</v>
       </c>
       <c r="B3" s="26">
         <v>3600</v>
       </c>
-      <c r="C3" s="26">
-        <v>0</v>
-      </c>
-      <c r="D3" s="26">
-        <v>0</v>
-      </c>
-      <c r="E3" s="26">
-        <v>-395127</v>
-      </c>
-      <c r="F3" s="26">
-        <v>0</v>
-      </c>
-      <c r="G3" s="26">
-        <v>0</v>
-      </c>
-      <c r="H3" s="26">
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>-395127.288299268</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
         <v>-3400000</v>
       </c>
-      <c r="I3" s="26">
-        <v>0</v>
-      </c>
-      <c r="J3" s="26">
+      <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="J3">
         <v>337520</v>
       </c>
-      <c r="K3" s="26">
-        <v>0</v>
-      </c>
-      <c r="L3" s="26">
-        <v>0</v>
-      </c>
-      <c r="M3" s="26">
-        <v>0</v>
-      </c>
-      <c r="N3" s="26">
-        <v>0</v>
-      </c>
-      <c r="O3" s="26">
-        <v>0</v>
-      </c>
-      <c r="P3" s="26">
+      <c r="K3">
+        <v>0</v>
+      </c>
+      <c r="L3">
+        <v>0</v>
+      </c>
+      <c r="M3">
+        <v>0</v>
+      </c>
+      <c r="N3">
+        <v>0</v>
+      </c>
+      <c r="O3">
+        <v>-62750</v>
+      </c>
+      <c r="P3">
         <v>0.5</v>
       </c>
-      <c r="Q3" s="26">
+      <c r="Q3">
         <v>0.5</v>
       </c>
-      <c r="R3" s="26">
-        <v>0.34861500000000001</v>
-      </c>
-      <c r="S3" s="26">
+      <c r="R3">
+        <v>0.34861478657396999</v>
+      </c>
+      <c r="S3">
         <v>0.5</v>
       </c>
-      <c r="T3" s="26">
-        <v>-3457607</v>
-      </c>
-      <c r="U3" s="26">
-        <v>0</v>
-      </c>
-      <c r="V3" s="26">
-        <v>0.235038</v>
-      </c>
-      <c r="W3" s="26">
+      <c r="T3">
+        <v>-3457607.28829927</v>
+      </c>
+      <c r="U3">
+        <v>-62750</v>
+      </c>
+      <c r="V3">
+        <v>0.23503848899999999</v>
+      </c>
+      <c r="W3">
         <v>0.17444999999999999</v>
       </c>
       <c r="X3" s="28">
         <f t="shared" ref="X3:X25" si="0">IF(T3&lt;0,T3,0)</f>
-        <v>-3457607</v>
+        <v>-3457607.28829927</v>
       </c>
       <c r="Y3" s="28">
         <f t="shared" ref="Y3:Y25" si="1">IF(T3&gt;0,T3,0)</f>
@@ -2866,7 +2855,7 @@
       </c>
       <c r="Z3" s="28">
         <f t="shared" ref="Z3:Z25" si="2">IF(U3&lt;0,U3,0)</f>
-        <v>0</v>
+        <v>-62750</v>
       </c>
       <c r="AA3" s="28">
         <f t="shared" ref="AA3:AA25" si="3">IF(U3&gt;0,U3,0)</f>
@@ -2882,7 +2871,7 @@
       </c>
       <c r="AD3" s="30">
         <f t="shared" ref="AD3:AD25" si="6">SUM(C3,D3,E3,F3,G3,H3,I3,J3,N3,O3,-X3,-Y3,-Z3,-AA3)</f>
-        <v>0</v>
+        <v>1.862645149230957E-9</v>
       </c>
       <c r="AE3" s="30">
         <f>IF('Day1'!A3&lt;KPI!$B$15,1,0)</f>
@@ -2893,87 +2882,87 @@
         <v>0</v>
       </c>
       <c r="AG3" s="30">
-        <f t="shared" ref="AG3:AG26" si="7">E3</f>
-        <v>-395127</v>
+        <f t="shared" ref="AG3:AG25" si="7">X3*AE3</f>
+        <v>-3457607.28829927</v>
       </c>
       <c r="AH3" s="30">
-        <f t="shared" ref="AH3:AH26" si="8">O3</f>
+        <f t="shared" ref="AH3:AH25" si="8">Y3*AF3</f>
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:34" x14ac:dyDescent="0.3">
-      <c r="A4" s="32">
+      <c r="A4" s="31">
         <v>0.25442999999999999</v>
       </c>
       <c r="B4" s="26">
         <v>7200</v>
       </c>
-      <c r="C4" s="26">
-        <v>0</v>
-      </c>
-      <c r="D4" s="26">
-        <v>0</v>
-      </c>
-      <c r="E4" s="26">
-        <v>-386839</v>
-      </c>
-      <c r="F4" s="26">
-        <v>0</v>
-      </c>
-      <c r="G4" s="26">
-        <v>0</v>
-      </c>
-      <c r="H4" s="26">
-        <v>0</v>
-      </c>
-      <c r="I4" s="26">
-        <v>0</v>
-      </c>
-      <c r="J4" s="26">
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>-386838.771823544</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+      <c r="J4">
         <v>337500</v>
       </c>
-      <c r="K4" s="26">
-        <v>0</v>
-      </c>
-      <c r="L4" s="26">
-        <v>0</v>
-      </c>
-      <c r="M4" s="26">
-        <v>0</v>
-      </c>
-      <c r="N4" s="26">
-        <v>0</v>
-      </c>
-      <c r="O4" s="26">
-        <v>0</v>
-      </c>
-      <c r="P4" s="26">
-        <v>0.83590699999999996</v>
-      </c>
-      <c r="Q4" s="26">
+      <c r="K4">
+        <v>0</v>
+      </c>
+      <c r="L4">
+        <v>0</v>
+      </c>
+      <c r="M4">
+        <v>0</v>
+      </c>
+      <c r="N4">
+        <v>0</v>
+      </c>
+      <c r="O4">
+        <v>-62750</v>
+      </c>
+      <c r="P4">
+        <v>0.83590706729170605</v>
+      </c>
+      <c r="Q4">
         <v>0.5</v>
       </c>
-      <c r="R4" s="26">
-        <v>0.14677000000000001</v>
-      </c>
-      <c r="S4" s="26">
+      <c r="R4">
+        <v>0.14676982881064499</v>
+      </c>
+      <c r="S4">
         <v>0.5</v>
       </c>
-      <c r="T4" s="26">
-        <v>-49338.8</v>
-      </c>
-      <c r="U4" s="26">
-        <v>0</v>
-      </c>
-      <c r="V4" s="26">
-        <v>0.20922399999999999</v>
-      </c>
-      <c r="W4" s="26">
+      <c r="T4">
+        <v>-49338.771823543502</v>
+      </c>
+      <c r="U4">
+        <v>-62750</v>
+      </c>
+      <c r="V4">
+        <v>0.20922375300000001</v>
+      </c>
+      <c r="W4">
         <v>0.14960999999999999</v>
       </c>
       <c r="X4" s="28">
         <f t="shared" si="0"/>
-        <v>-49338.8</v>
+        <v>-49338.771823543502</v>
       </c>
       <c r="Y4" s="28">
         <f t="shared" si="1"/>
@@ -2981,7 +2970,7 @@
       </c>
       <c r="Z4" s="28">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>-62750</v>
       </c>
       <c r="AA4" s="28">
         <f t="shared" si="3"/>
@@ -2989,7 +2978,7 @@
       </c>
       <c r="AB4" s="30">
         <f t="shared" si="4"/>
-        <v>-0.19999999999708962</v>
+        <v>-4.9476511776447296E-10</v>
       </c>
       <c r="AC4" s="30">
         <f t="shared" si="5"/>
@@ -2997,7 +2986,7 @@
       </c>
       <c r="AD4" s="30">
         <f>SUM(C4,D4,E4,F4,G4,H4,I4,J4,N4,O4,-X4,-Y4,-Z4,-AA4)</f>
-        <v>-0.19999999999708962</v>
+        <v>-4.9476511776447296E-10</v>
       </c>
       <c r="AE4" s="30">
         <f>IF('Day1'!A4&lt;KPI!$B$15,1,0)</f>
@@ -3009,7 +2998,7 @@
       </c>
       <c r="AG4" s="30">
         <f t="shared" si="7"/>
-        <v>-386839</v>
+        <v>-49338.771823543502</v>
       </c>
       <c r="AH4" s="30">
         <f t="shared" si="8"/>
@@ -3017,78 +3006,78 @@
       </c>
     </row>
     <row r="5" spans="1:34" x14ac:dyDescent="0.3">
-      <c r="A5" s="32">
+      <c r="A5" s="31">
         <v>0.25297999999999998</v>
       </c>
       <c r="B5" s="26">
         <v>10800</v>
       </c>
-      <c r="C5" s="26">
-        <v>0</v>
-      </c>
-      <c r="D5" s="26">
-        <v>0</v>
-      </c>
-      <c r="E5" s="26">
-        <v>-400328</v>
-      </c>
-      <c r="F5" s="26">
-        <v>0</v>
-      </c>
-      <c r="G5" s="26">
-        <v>0</v>
-      </c>
-      <c r="H5" s="26">
-        <v>0</v>
-      </c>
-      <c r="I5" s="26">
-        <v>0</v>
-      </c>
-      <c r="J5" s="26">
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>-400327.600799268</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="J5">
         <v>337500</v>
       </c>
-      <c r="K5" s="26">
-        <v>0</v>
-      </c>
-      <c r="L5" s="26">
-        <v>0</v>
-      </c>
-      <c r="M5" s="26">
-        <v>0</v>
-      </c>
-      <c r="N5" s="26">
-        <v>0</v>
-      </c>
-      <c r="O5" s="26">
-        <v>0</v>
-      </c>
-      <c r="P5" s="26">
-        <v>0.83590699999999996</v>
-      </c>
-      <c r="Q5" s="26">
+      <c r="K5">
+        <v>0</v>
+      </c>
+      <c r="L5">
+        <v>0</v>
+      </c>
+      <c r="M5">
+        <v>0</v>
+      </c>
+      <c r="N5">
+        <v>0</v>
+      </c>
+      <c r="O5">
+        <v>-62750</v>
+      </c>
+      <c r="P5">
+        <v>0.83590706729170605</v>
+      </c>
+      <c r="Q5">
         <v>0.5</v>
       </c>
-      <c r="R5" s="26">
-        <v>3.4637000000000001E-2</v>
-      </c>
-      <c r="S5" s="26">
+      <c r="R5">
+        <v>3.46370636166555E-2</v>
+      </c>
+      <c r="S5">
         <v>0.5</v>
       </c>
-      <c r="T5" s="26">
-        <v>-62827.6</v>
-      </c>
-      <c r="U5" s="26">
-        <v>0</v>
-      </c>
-      <c r="V5" s="26">
-        <v>0.200679</v>
-      </c>
-      <c r="W5" s="26">
+      <c r="T5">
+        <v>-62827.600799268097</v>
+      </c>
+      <c r="U5">
+        <v>-62750</v>
+      </c>
+      <c r="V5">
+        <v>0.200678984</v>
+      </c>
+      <c r="W5">
         <v>0.14057</v>
       </c>
       <c r="X5" s="28">
         <f t="shared" si="0"/>
-        <v>-62827.6</v>
+        <v>-62827.600799268097</v>
       </c>
       <c r="Y5" s="28">
         <f t="shared" si="1"/>
@@ -3096,7 +3085,7 @@
       </c>
       <c r="Z5" s="28">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>-62750</v>
       </c>
       <c r="AA5" s="28">
         <f>IF(U5&gt;0,U5,0)</f>
@@ -3104,7 +3093,7 @@
       </c>
       <c r="AB5" s="30">
         <f t="shared" si="4"/>
-        <v>-0.40000000000145519</v>
+        <v>1.0186340659856796E-10</v>
       </c>
       <c r="AC5" s="30">
         <f t="shared" si="5"/>
@@ -3112,7 +3101,7 @@
       </c>
       <c r="AD5" s="30">
         <f t="shared" si="6"/>
-        <v>-0.40000000000145519</v>
+        <v>1.0186340659856796E-10</v>
       </c>
       <c r="AE5" s="30">
         <f>IF('Day1'!A5&lt;KPI!$B$15,1,0)</f>
@@ -3124,7 +3113,7 @@
       </c>
       <c r="AG5" s="30">
         <f t="shared" si="7"/>
-        <v>-400328</v>
+        <v>-62827.600799268097</v>
       </c>
       <c r="AH5" s="30">
         <f t="shared" si="8"/>
@@ -3132,78 +3121,78 @@
       </c>
     </row>
     <row r="6" spans="1:34" x14ac:dyDescent="0.3">
-      <c r="A6" s="32">
+      <c r="A6" s="31">
         <v>0.25274999999999997</v>
       </c>
       <c r="B6" s="26">
         <v>14400</v>
       </c>
-      <c r="C6" s="26">
-        <v>0</v>
-      </c>
-      <c r="D6" s="26">
-        <v>0</v>
-      </c>
-      <c r="E6" s="26">
-        <v>-398289</v>
-      </c>
-      <c r="F6" s="26">
-        <v>0</v>
-      </c>
-      <c r="G6" s="26">
-        <v>0</v>
-      </c>
-      <c r="H6" s="26">
-        <v>0</v>
-      </c>
-      <c r="I6" s="26">
-        <v>0</v>
-      </c>
-      <c r="J6" s="26">
-        <v>0</v>
-      </c>
-      <c r="K6" s="26">
-        <v>0</v>
-      </c>
-      <c r="L6" s="26">
-        <v>0</v>
-      </c>
-      <c r="M6" s="26">
-        <v>0</v>
-      </c>
-      <c r="N6" s="26">
-        <v>0</v>
-      </c>
-      <c r="O6" s="26">
-        <v>0</v>
-      </c>
-      <c r="P6" s="26">
-        <v>0.83590699999999996</v>
-      </c>
-      <c r="Q6" s="26">
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>-398289.084323544</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
+      <c r="K6">
+        <v>0</v>
+      </c>
+      <c r="L6">
+        <v>0</v>
+      </c>
+      <c r="M6">
+        <v>0</v>
+      </c>
+      <c r="N6">
+        <v>0</v>
+      </c>
+      <c r="O6">
+        <v>-62750</v>
+      </c>
+      <c r="P6">
+        <v>0.83590706729170605</v>
+      </c>
+      <c r="Q6">
         <v>0.5</v>
       </c>
-      <c r="R6" s="26">
-        <v>0</v>
-      </c>
-      <c r="S6" s="26">
+      <c r="R6">
+        <v>0</v>
+      </c>
+      <c r="S6">
         <v>0.5</v>
       </c>
-      <c r="T6" s="26">
-        <v>-398289</v>
-      </c>
-      <c r="U6" s="26">
-        <v>0</v>
-      </c>
-      <c r="V6" s="26">
-        <v>0.20197599999999999</v>
-      </c>
-      <c r="W6" s="26">
+      <c r="T6">
+        <v>-398289.084323544</v>
+      </c>
+      <c r="U6">
+        <v>-62750</v>
+      </c>
+      <c r="V6">
+        <v>0.20197621599999999</v>
+      </c>
+      <c r="W6">
         <v>0.14055999999999999</v>
       </c>
       <c r="X6" s="28">
         <f t="shared" si="0"/>
-        <v>-398289</v>
+        <v>-398289.084323544</v>
       </c>
       <c r="Y6" s="28">
         <f t="shared" si="1"/>
@@ -3211,7 +3200,7 @@
       </c>
       <c r="Z6" s="28">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>-62750</v>
       </c>
       <c r="AA6" s="28">
         <f t="shared" si="3"/>
@@ -3239,7 +3228,7 @@
       </c>
       <c r="AG6" s="30">
         <f t="shared" si="7"/>
-        <v>-398289</v>
+        <v>-398289.084323544</v>
       </c>
       <c r="AH6" s="30">
         <f t="shared" si="8"/>
@@ -3247,78 +3236,78 @@
       </c>
     </row>
     <row r="7" spans="1:34" x14ac:dyDescent="0.3">
-      <c r="A7" s="32">
+      <c r="A7" s="31">
         <v>0.25497999999999998</v>
       </c>
       <c r="B7" s="26">
         <v>18000</v>
       </c>
-      <c r="C7" s="26">
-        <v>0</v>
-      </c>
-      <c r="D7" s="26">
-        <v>0</v>
-      </c>
-      <c r="E7" s="26">
-        <v>-485746</v>
-      </c>
-      <c r="F7" s="26">
-        <v>0</v>
-      </c>
-      <c r="G7" s="26">
-        <v>0</v>
-      </c>
-      <c r="H7" s="26">
-        <v>0</v>
-      </c>
-      <c r="I7" s="26">
-        <v>0</v>
-      </c>
-      <c r="J7" s="26">
-        <v>0</v>
-      </c>
-      <c r="K7" s="26">
-        <v>0</v>
-      </c>
-      <c r="L7" s="26">
-        <v>0</v>
-      </c>
-      <c r="M7" s="26">
-        <v>0</v>
-      </c>
-      <c r="N7" s="26">
-        <v>0</v>
-      </c>
-      <c r="O7" s="26">
-        <v>-2634.3</v>
-      </c>
-      <c r="P7" s="26">
-        <v>0.83590699999999996</v>
-      </c>
-      <c r="Q7" s="26">
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>-485746.16169024498</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
+      <c r="J7">
+        <v>0</v>
+      </c>
+      <c r="K7">
+        <v>0</v>
+      </c>
+      <c r="L7">
+        <v>0</v>
+      </c>
+      <c r="M7">
+        <v>0</v>
+      </c>
+      <c r="N7">
+        <v>0</v>
+      </c>
+      <c r="O7">
+        <v>-89092.975206611591</v>
+      </c>
+      <c r="P7">
+        <v>0.83590706729170605</v>
+      </c>
+      <c r="Q7">
         <v>0.5</v>
       </c>
-      <c r="R7" s="26">
-        <v>0</v>
-      </c>
-      <c r="S7" s="26">
+      <c r="R7">
+        <v>0</v>
+      </c>
+      <c r="S7">
         <v>0.5</v>
       </c>
-      <c r="T7" s="26">
-        <v>-485746</v>
-      </c>
-      <c r="U7" s="26">
-        <v>-2634.3</v>
-      </c>
-      <c r="V7" s="26">
-        <v>0.20758399999999999</v>
-      </c>
-      <c r="W7" s="26">
+      <c r="T7">
+        <v>-485746.16169024498</v>
+      </c>
+      <c r="U7">
+        <v>-89092.975206611605</v>
+      </c>
+      <c r="V7">
+        <v>0.20758394199999999</v>
+      </c>
+      <c r="W7">
         <v>0.14516000000000001</v>
       </c>
       <c r="X7" s="28">
         <f t="shared" si="0"/>
-        <v>-485746</v>
+        <v>-485746.16169024498</v>
       </c>
       <c r="Y7" s="28">
         <f t="shared" si="1"/>
@@ -3326,7 +3315,7 @@
       </c>
       <c r="Z7" s="28">
         <f t="shared" si="2"/>
-        <v>-2634.3</v>
+        <v>-89092.975206611605</v>
       </c>
       <c r="AA7" s="28">
         <f t="shared" si="3"/>
@@ -3342,7 +3331,7 @@
       </c>
       <c r="AD7" s="30">
         <f t="shared" si="6"/>
-        <v>1.1823431123048067E-11</v>
+        <v>-1.4551915228366852E-11</v>
       </c>
       <c r="AE7" s="30">
         <f>IF('Day1'!A7&lt;KPI!$B$15,1,0)</f>
@@ -3354,86 +3343,86 @@
       </c>
       <c r="AG7" s="30">
         <f t="shared" si="7"/>
-        <v>-485746</v>
+        <v>-485746.16169024498</v>
       </c>
       <c r="AH7" s="30">
         <f t="shared" si="8"/>
-        <v>-2634.3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:34" x14ac:dyDescent="0.3">
-      <c r="A8" s="32">
+      <c r="A8" s="31">
         <v>0.26271</v>
       </c>
       <c r="B8" s="26">
         <v>21600</v>
       </c>
-      <c r="C8" s="26">
-        <v>0</v>
-      </c>
-      <c r="D8" s="26">
-        <v>0</v>
-      </c>
-      <c r="E8" s="26">
-        <v>-487657</v>
-      </c>
-      <c r="F8" s="26">
-        <v>0</v>
-      </c>
-      <c r="G8" s="26">
-        <v>0</v>
-      </c>
-      <c r="H8" s="26">
-        <v>0</v>
-      </c>
-      <c r="I8" s="26">
-        <v>0</v>
-      </c>
-      <c r="J8" s="26">
-        <v>0</v>
-      </c>
-      <c r="K8" s="26">
-        <v>0</v>
-      </c>
-      <c r="L8" s="26">
-        <v>0</v>
-      </c>
-      <c r="M8" s="26">
-        <v>0</v>
-      </c>
-      <c r="N8" s="26">
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>-487656.94417347398</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>0</v>
+      </c>
+      <c r="J8">
+        <v>0</v>
+      </c>
+      <c r="K8">
+        <v>0</v>
+      </c>
+      <c r="L8">
+        <v>0</v>
+      </c>
+      <c r="M8">
+        <v>0</v>
+      </c>
+      <c r="N8">
         <v>-187900</v>
       </c>
-      <c r="O8" s="26">
-        <v>-5268.6</v>
-      </c>
-      <c r="P8" s="26">
-        <v>0.83590699999999996</v>
-      </c>
-      <c r="Q8" s="26">
+      <c r="O8">
+        <v>-608333.34516176383</v>
+      </c>
+      <c r="P8">
+        <v>0.83590706729170605</v>
+      </c>
+      <c r="Q8">
         <v>0.5</v>
       </c>
-      <c r="R8" s="26">
-        <v>0</v>
-      </c>
-      <c r="S8" s="26">
-        <v>0.54529099999999997</v>
-      </c>
-      <c r="T8" s="26">
-        <v>-487657</v>
-      </c>
-      <c r="U8" s="26">
-        <v>-193169</v>
-      </c>
-      <c r="V8" s="26">
-        <v>0.222909</v>
-      </c>
-      <c r="W8" s="26">
+      <c r="R8">
+        <v>0</v>
+      </c>
+      <c r="S8">
+        <v>0.54529064105901504</v>
+      </c>
+      <c r="T8">
+        <v>-487656.94417347398</v>
+      </c>
+      <c r="U8">
+        <v>-796233.345161765</v>
+      </c>
+      <c r="V8">
+        <v>0.22290945400000001</v>
+      </c>
+      <c r="W8">
         <v>0.15945999999999999</v>
       </c>
       <c r="X8" s="28">
         <f t="shared" si="0"/>
-        <v>-487657</v>
+        <v>-487656.94417347398</v>
       </c>
       <c r="Y8" s="28">
         <f t="shared" si="1"/>
@@ -3441,7 +3430,7 @@
       </c>
       <c r="Z8" s="28">
         <f t="shared" si="2"/>
-        <v>-193169</v>
+        <v>-796233.345161765</v>
       </c>
       <c r="AA8" s="28">
         <f t="shared" si="3"/>
@@ -3453,11 +3442,11 @@
       </c>
       <c r="AC8" s="30">
         <f t="shared" si="5"/>
-        <v>0.39999999999417923</v>
+        <v>1.1641532182693481E-9</v>
       </c>
       <c r="AD8" s="30">
         <f t="shared" si="6"/>
-        <v>0.40000000002328306</v>
+        <v>1.1641532182693481E-9</v>
       </c>
       <c r="AE8" s="30">
         <f>IF('Day1'!A8&lt;KPI!$B$15,1,0)</f>
@@ -3469,86 +3458,86 @@
       </c>
       <c r="AG8" s="30">
         <f t="shared" si="7"/>
-        <v>-487657</v>
+        <v>-487656.94417347398</v>
       </c>
       <c r="AH8" s="30">
         <f t="shared" si="8"/>
-        <v>-5268.6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:34" x14ac:dyDescent="0.3">
-      <c r="A9" s="32">
+      <c r="A9" s="31">
         <v>0.269783</v>
       </c>
       <c r="B9" s="26">
         <v>25200</v>
       </c>
-      <c r="C9" s="26">
-        <v>0</v>
-      </c>
-      <c r="D9" s="26">
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
         <v>1112.5</v>
       </c>
-      <c r="E9" s="26">
-        <v>-515761</v>
-      </c>
-      <c r="F9" s="26">
-        <v>0</v>
-      </c>
-      <c r="G9" s="26">
-        <v>0</v>
-      </c>
-      <c r="H9" s="26">
-        <v>0</v>
-      </c>
-      <c r="I9" s="26">
-        <v>0</v>
-      </c>
-      <c r="J9" s="26">
+      <c r="E9">
+        <v>-515761.03260860901</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <v>0</v>
+      </c>
+      <c r="J9">
         <v>-337500</v>
       </c>
-      <c r="K9" s="26">
-        <v>0</v>
-      </c>
-      <c r="L9" s="26">
-        <v>0</v>
-      </c>
-      <c r="M9" s="26">
-        <v>0</v>
-      </c>
-      <c r="N9" s="26">
+      <c r="K9">
+        <v>0</v>
+      </c>
+      <c r="L9">
+        <v>0</v>
+      </c>
+      <c r="M9">
+        <v>0</v>
+      </c>
+      <c r="N9">
         <v>-81800</v>
       </c>
-      <c r="O9" s="26">
-        <v>-13171.5</v>
-      </c>
-      <c r="P9" s="26">
-        <v>0.83590699999999996</v>
-      </c>
-      <c r="Q9" s="26">
+      <c r="O9">
+        <v>-1032778.9374482664</v>
+      </c>
+      <c r="P9">
+        <v>0.83590706729170605</v>
+      </c>
+      <c r="Q9">
         <v>0.5</v>
       </c>
-      <c r="R9" s="26">
-        <v>0</v>
-      </c>
-      <c r="S9" s="26">
-        <v>0.56500700000000004</v>
-      </c>
-      <c r="T9" s="26">
-        <v>-852149</v>
-      </c>
-      <c r="U9" s="26">
-        <v>-94971.5</v>
-      </c>
-      <c r="V9" s="26">
-        <v>0.23400599999999999</v>
-      </c>
-      <c r="W9" s="26">
+      <c r="R9">
+        <v>0</v>
+      </c>
+      <c r="S9">
+        <v>0.56500737569779902</v>
+      </c>
+      <c r="T9">
+        <v>-852148.53260860895</v>
+      </c>
+      <c r="U9">
+        <v>-1114578.9374482699</v>
+      </c>
+      <c r="V9">
+        <v>0.23400607000000001</v>
+      </c>
+      <c r="W9">
         <v>0.17157</v>
       </c>
       <c r="X9" s="28">
         <f t="shared" si="0"/>
-        <v>-852149</v>
+        <v>-852148.53260860895</v>
       </c>
       <c r="Y9" s="28">
         <f t="shared" si="1"/>
@@ -3556,7 +3545,7 @@
       </c>
       <c r="Z9" s="28">
         <f t="shared" si="2"/>
-        <v>-94971.5</v>
+        <v>-1114578.9374482699</v>
       </c>
       <c r="AA9" s="28">
         <f t="shared" si="3"/>
@@ -3564,15 +3553,15 @@
       </c>
       <c r="AB9" s="30">
         <f t="shared" si="4"/>
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="AC9" s="30">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>3.4924596548080444E-9</v>
       </c>
       <c r="AD9" s="30">
         <f t="shared" si="6"/>
-        <v>0.5</v>
+        <v>3.4924596548080444E-9</v>
       </c>
       <c r="AE9" s="30">
         <f>IF('Day1'!A9&lt;KPI!$B$15,1,0)</f>
@@ -3584,86 +3573,86 @@
       </c>
       <c r="AG9" s="30">
         <f t="shared" si="7"/>
-        <v>-515761</v>
+        <v>0</v>
       </c>
       <c r="AH9" s="30">
         <f t="shared" si="8"/>
-        <v>-13171.5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:34" x14ac:dyDescent="0.3">
-      <c r="A10" s="32">
+      <c r="A10" s="31">
         <v>0.27707500000000002</v>
       </c>
       <c r="B10" s="26">
         <v>28800</v>
       </c>
-      <c r="C10" s="26">
-        <v>0</v>
-      </c>
-      <c r="D10" s="26">
-        <v>287081.3</v>
-      </c>
-      <c r="E10" s="26">
-        <v>-559946</v>
-      </c>
-      <c r="F10" s="26">
-        <v>0</v>
-      </c>
-      <c r="G10" s="26">
-        <v>0</v>
-      </c>
-      <c r="H10" s="26">
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>287081.25</v>
+      </c>
+      <c r="E10">
+        <v>-559945.91599036905</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10">
         <v>142600</v>
       </c>
-      <c r="I10" s="26">
-        <v>0</v>
-      </c>
-      <c r="J10" s="26">
+      <c r="I10">
+        <v>0</v>
+      </c>
+      <c r="J10">
         <v>-337500</v>
       </c>
-      <c r="K10" s="26">
-        <v>0</v>
-      </c>
-      <c r="L10" s="26">
-        <v>0</v>
-      </c>
-      <c r="M10" s="26">
-        <v>0</v>
-      </c>
-      <c r="N10" s="26">
+      <c r="K10">
+        <v>0</v>
+      </c>
+      <c r="L10">
+        <v>0</v>
+      </c>
+      <c r="M10">
+        <v>0</v>
+      </c>
+      <c r="N10">
         <v>-78020</v>
       </c>
-      <c r="O10" s="26">
-        <v>-5268.6</v>
-      </c>
-      <c r="P10" s="26">
-        <v>0.83590699999999996</v>
-      </c>
-      <c r="Q10" s="26">
+      <c r="O10">
+        <v>-1047916.6784950979</v>
+      </c>
+      <c r="P10">
+        <v>0.83590706729170605</v>
+      </c>
+      <c r="Q10">
         <v>0.5</v>
       </c>
-      <c r="R10" s="26">
-        <v>4.3049999999999998E-3</v>
-      </c>
-      <c r="S10" s="26">
-        <v>0.58381300000000003</v>
-      </c>
-      <c r="T10" s="26">
-        <v>-467765</v>
-      </c>
-      <c r="U10" s="26">
-        <v>-83288.600000000006</v>
-      </c>
-      <c r="V10" s="26">
-        <v>0.204595</v>
-      </c>
-      <c r="W10" s="26">
+      <c r="R10">
+        <v>4.3051506316812401E-3</v>
+      </c>
+      <c r="S10">
+        <v>0.58381299472613502</v>
+      </c>
+      <c r="T10">
+        <v>-467764.66599036899</v>
+      </c>
+      <c r="U10">
+        <v>-1125936.6784951</v>
+      </c>
+      <c r="V10">
+        <v>0.20459496199999999</v>
+      </c>
+      <c r="W10">
         <v>0.14926</v>
       </c>
       <c r="X10" s="28">
         <f t="shared" si="0"/>
-        <v>-467765</v>
+        <v>-467764.66599036899</v>
       </c>
       <c r="Y10" s="28">
         <f t="shared" si="1"/>
@@ -3671,7 +3660,7 @@
       </c>
       <c r="Z10" s="28">
         <f t="shared" si="2"/>
-        <v>-83288.600000000006</v>
+        <v>-1125936.6784951</v>
       </c>
       <c r="AA10" s="28">
         <f t="shared" si="3"/>
@@ -3679,15 +3668,15 @@
       </c>
       <c r="AB10" s="30">
         <f t="shared" si="4"/>
-        <v>0.30000000004656613</v>
+        <v>0</v>
       </c>
       <c r="AC10" s="30">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>2.0954757928848267E-9</v>
       </c>
       <c r="AD10" s="30">
         <f t="shared" si="6"/>
-        <v>0.30000000007566996</v>
+        <v>2.0954757928848267E-9</v>
       </c>
       <c r="AE10" s="30">
         <f>IF('Day1'!A10&lt;KPI!$B$15,1,0)</f>
@@ -3699,81 +3688,81 @@
       </c>
       <c r="AG10" s="30">
         <f t="shared" si="7"/>
-        <v>-559946</v>
+        <v>0</v>
       </c>
       <c r="AH10" s="30">
         <f t="shared" si="8"/>
-        <v>-5268.6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:34" x14ac:dyDescent="0.3">
-      <c r="A11" s="32">
+      <c r="A11" s="31">
         <v>0.27672799999999997</v>
       </c>
       <c r="B11" s="26">
         <v>32400</v>
       </c>
-      <c r="C11" s="26">
-        <v>0</v>
-      </c>
-      <c r="D11" s="26">
-        <v>1049419</v>
-      </c>
-      <c r="E11" s="26">
-        <v>-571927</v>
-      </c>
-      <c r="F11" s="26">
-        <v>0</v>
-      </c>
-      <c r="G11" s="26">
-        <v>0</v>
-      </c>
-      <c r="H11" s="26">
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>1049418.75</v>
+      </c>
+      <c r="E11">
+        <v>-571927.48888726695</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
         <v>815681.3</v>
       </c>
-      <c r="I11" s="26">
-        <v>0</v>
-      </c>
-      <c r="J11" s="26">
+      <c r="I11">
+        <v>0</v>
+      </c>
+      <c r="J11">
         <v>-212625</v>
       </c>
-      <c r="K11" s="26">
-        <v>0</v>
-      </c>
-      <c r="L11" s="26">
-        <v>0</v>
-      </c>
-      <c r="M11" s="26">
-        <v>0</v>
-      </c>
-      <c r="N11" s="26">
+      <c r="K11">
+        <v>0</v>
+      </c>
+      <c r="L11">
+        <v>0</v>
+      </c>
+      <c r="M11">
+        <v>0</v>
+      </c>
+      <c r="N11">
         <v>-125565</v>
       </c>
-      <c r="O11" s="26">
-        <v>-1317.15</v>
-      </c>
-      <c r="P11" s="26">
-        <v>0.81646099999999999</v>
-      </c>
-      <c r="Q11" s="26">
+      <c r="O11">
+        <v>-857735.54901851318</v>
+      </c>
+      <c r="P11">
+        <v>0.81646119790012395</v>
+      </c>
+      <c r="Q11">
         <v>0.5</v>
       </c>
-      <c r="R11" s="26">
-        <v>7.3805999999999997E-2</v>
-      </c>
-      <c r="S11" s="26">
-        <v>0.61407900000000004</v>
-      </c>
-      <c r="T11" s="26">
-        <v>1080548</v>
-      </c>
-      <c r="U11" s="26">
-        <v>-126882</v>
-      </c>
-      <c r="V11" s="26">
-        <v>0.19017899999999999</v>
-      </c>
-      <c r="W11" s="26">
+      <c r="R11">
+        <v>7.3805879494654905E-2</v>
+      </c>
+      <c r="S11">
+        <v>0.61407866446841897</v>
+      </c>
+      <c r="T11">
+        <v>1080547.5611127301</v>
+      </c>
+      <c r="U11">
+        <v>-983300.54901851504</v>
+      </c>
+      <c r="V11">
+        <v>0.19017879100000001</v>
+      </c>
+      <c r="W11">
         <v>0.14055999999999999</v>
       </c>
       <c r="X11" s="28">
@@ -3782,11 +3771,11 @@
       </c>
       <c r="Y11" s="28">
         <f t="shared" si="1"/>
-        <v>1080548</v>
+        <v>1080547.5611127301</v>
       </c>
       <c r="Z11" s="28">
         <f t="shared" si="2"/>
-        <v>-126882</v>
+        <v>-983300.54901851504</v>
       </c>
       <c r="AA11" s="28">
         <f t="shared" si="3"/>
@@ -3794,15 +3783,15 @@
       </c>
       <c r="AB11" s="30">
         <f t="shared" si="4"/>
-        <v>0.30000000004656613</v>
+        <v>3.0267983675003052E-9</v>
       </c>
       <c r="AC11" s="30">
         <f t="shared" si="5"/>
-        <v>-0.14999999999417923</v>
+        <v>1.862645149230957E-9</v>
       </c>
       <c r="AD11" s="30">
         <f t="shared" si="6"/>
-        <v>0.15000000002328306</v>
+        <v>4.8894435167312622E-9</v>
       </c>
       <c r="AE11" s="30">
         <f>IF('Day1'!A11&lt;KPI!$B$15,1,0)</f>
@@ -3814,81 +3803,81 @@
       </c>
       <c r="AG11" s="30">
         <f t="shared" si="7"/>
-        <v>-571927</v>
+        <v>0</v>
       </c>
       <c r="AH11" s="30">
         <f t="shared" si="8"/>
-        <v>-1317.15</v>
+        <v>1080547.5611127301</v>
       </c>
     </row>
     <row r="12" spans="1:34" x14ac:dyDescent="0.3">
-      <c r="A12" s="32">
+      <c r="A12" s="31">
         <v>0.27678199999999997</v>
       </c>
       <c r="B12" s="26">
         <v>36000</v>
       </c>
-      <c r="C12" s="26">
-        <v>0</v>
-      </c>
-      <c r="D12" s="26">
-        <v>1648938</v>
-      </c>
-      <c r="E12" s="26">
-        <v>-544977</v>
-      </c>
-      <c r="F12" s="26">
-        <v>0</v>
-      </c>
-      <c r="G12" s="26">
-        <v>0</v>
-      </c>
-      <c r="H12" s="26">
-        <v>1257936</v>
-      </c>
-      <c r="I12" s="26">
-        <v>0</v>
-      </c>
-      <c r="J12" s="26">
-        <v>0</v>
-      </c>
-      <c r="K12" s="26">
-        <v>0</v>
-      </c>
-      <c r="L12" s="26">
-        <v>0</v>
-      </c>
-      <c r="M12" s="26">
-        <v>0</v>
-      </c>
-      <c r="N12" s="26">
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>1648937.5</v>
+      </c>
+      <c r="E12">
+        <v>-544977.19768498605</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <v>1257935.7</v>
+      </c>
+      <c r="I12">
+        <v>0</v>
+      </c>
+      <c r="J12">
+        <v>0</v>
+      </c>
+      <c r="K12">
+        <v>0</v>
+      </c>
+      <c r="L12">
+        <v>0</v>
+      </c>
+      <c r="M12">
+        <v>0</v>
+      </c>
+      <c r="N12">
         <v>-153975</v>
       </c>
-      <c r="O12" s="26">
-        <v>0</v>
-      </c>
-      <c r="P12" s="26">
-        <v>0.70525000000000004</v>
-      </c>
-      <c r="Q12" s="26">
+      <c r="O12">
+        <v>-744064.06141520804</v>
+      </c>
+      <c r="P12">
+        <v>0.70524996317869404</v>
+      </c>
+      <c r="Q12">
         <v>0.5</v>
       </c>
-      <c r="R12" s="26">
-        <v>0.10066799999999999</v>
-      </c>
-      <c r="S12" s="26">
-        <v>0.65119199999999999</v>
-      </c>
-      <c r="T12" s="26">
-        <v>2361896</v>
-      </c>
-      <c r="U12" s="26">
-        <v>-153975</v>
-      </c>
-      <c r="V12" s="26">
-        <v>0.17811399999999999</v>
-      </c>
-      <c r="W12" s="26">
+      <c r="R12">
+        <v>0.10066812439261399</v>
+      </c>
+      <c r="S12">
+        <v>0.65119216344160702</v>
+      </c>
+      <c r="T12">
+        <v>2361896.0023150099</v>
+      </c>
+      <c r="U12">
+        <v>-898039.06141520804</v>
+      </c>
+      <c r="V12">
+        <v>0.178113509</v>
+      </c>
+      <c r="W12">
         <v>0.13582</v>
       </c>
       <c r="X12" s="28">
@@ -3897,11 +3886,11 @@
       </c>
       <c r="Y12" s="28">
         <f t="shared" si="1"/>
-        <v>2361896</v>
+        <v>2361896.0023150099</v>
       </c>
       <c r="Z12" s="28">
         <f t="shared" si="2"/>
-        <v>-153975</v>
+        <v>-898039.06141520804</v>
       </c>
       <c r="AA12" s="28">
         <f t="shared" si="3"/>
@@ -3909,7 +3898,7 @@
       </c>
       <c r="AB12" s="30">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>3.7252902984619141E-9</v>
       </c>
       <c r="AC12" s="30">
         <f t="shared" si="5"/>
@@ -3917,7 +3906,7 @@
       </c>
       <c r="AD12" s="30">
         <f t="shared" si="6"/>
-        <v>1</v>
+        <v>3.7252902984619141E-9</v>
       </c>
       <c r="AE12" s="30">
         <f>IF('Day1'!A12&lt;KPI!$B$15,1,0)</f>
@@ -3929,81 +3918,81 @@
       </c>
       <c r="AG12" s="30">
         <f t="shared" si="7"/>
-        <v>-544977</v>
+        <v>0</v>
       </c>
       <c r="AH12" s="30">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>2361896.0023150099</v>
       </c>
     </row>
     <row r="13" spans="1:34" x14ac:dyDescent="0.3">
-      <c r="A13" s="32">
+      <c r="A13" s="31">
         <v>0.270368</v>
       </c>
       <c r="B13" s="26">
         <v>39600</v>
       </c>
-      <c r="C13" s="26">
-        <v>0</v>
-      </c>
-      <c r="D13" s="26">
-        <v>1230288</v>
-      </c>
-      <c r="E13" s="26">
-        <v>-505042</v>
-      </c>
-      <c r="F13" s="26">
-        <v>0</v>
-      </c>
-      <c r="G13" s="26">
-        <v>0</v>
-      </c>
-      <c r="H13" s="26">
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>1230287.5</v>
+      </c>
+      <c r="E13">
+        <v>-505042.41234859498</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+      <c r="H13">
         <v>874245</v>
       </c>
-      <c r="I13" s="26">
-        <v>0</v>
-      </c>
-      <c r="J13" s="26">
-        <v>0</v>
-      </c>
-      <c r="K13" s="26">
-        <v>0</v>
-      </c>
-      <c r="L13" s="26">
-        <v>0</v>
-      </c>
-      <c r="M13" s="26">
-        <v>0</v>
-      </c>
-      <c r="N13" s="26">
+      <c r="I13">
+        <v>0</v>
+      </c>
+      <c r="J13">
+        <v>0</v>
+      </c>
+      <c r="K13">
+        <v>0</v>
+      </c>
+      <c r="L13">
+        <v>0</v>
+      </c>
+      <c r="M13">
+        <v>0</v>
+      </c>
+      <c r="N13">
         <v>-149000</v>
       </c>
-      <c r="O13" s="26">
-        <v>0</v>
-      </c>
-      <c r="P13" s="26">
-        <v>0.53289200000000003</v>
-      </c>
-      <c r="Q13" s="26">
+      <c r="O13">
+        <v>-763975.76980124996</v>
+      </c>
+      <c r="P13">
+        <v>0.53289155218098105</v>
+      </c>
+      <c r="Q13">
         <v>0.5</v>
       </c>
-      <c r="R13" s="26">
-        <v>0.10066799999999999</v>
-      </c>
-      <c r="S13" s="26">
-        <v>0.68710700000000002</v>
-      </c>
-      <c r="T13" s="26">
-        <v>1599490</v>
-      </c>
-      <c r="U13" s="26">
-        <v>-149000</v>
-      </c>
-      <c r="V13" s="26">
-        <v>0.17130300000000001</v>
-      </c>
-      <c r="W13" s="26">
+      <c r="R13">
+        <v>0.10066812439261399</v>
+      </c>
+      <c r="S13">
+        <v>0.68710650893278902</v>
+      </c>
+      <c r="T13">
+        <v>1599490.0876514099</v>
+      </c>
+      <c r="U13">
+        <v>-912975.76980124996</v>
+      </c>
+      <c r="V13">
+        <v>0.171302914</v>
+      </c>
+      <c r="W13">
         <v>0.13022</v>
       </c>
       <c r="X13" s="28">
@@ -4012,11 +4001,11 @@
       </c>
       <c r="Y13" s="28">
         <f t="shared" si="1"/>
-        <v>1599490</v>
+        <v>1599490.0876514099</v>
       </c>
       <c r="Z13" s="28">
         <f t="shared" si="2"/>
-        <v>-149000</v>
+        <v>-912975.76980124996</v>
       </c>
       <c r="AA13" s="28">
         <f t="shared" si="3"/>
@@ -4024,7 +4013,7 @@
       </c>
       <c r="AB13" s="30">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>-4.8894435167312622E-9</v>
       </c>
       <c r="AC13" s="30">
         <f t="shared" si="5"/>
@@ -4032,7 +4021,7 @@
       </c>
       <c r="AD13" s="30">
         <f t="shared" si="6"/>
-        <v>1</v>
+        <v>-4.8894435167312622E-9</v>
       </c>
       <c r="AE13" s="30">
         <f>IF('Day1'!A13&lt;KPI!$B$15,1,0)</f>
@@ -4044,81 +4033,81 @@
       </c>
       <c r="AG13" s="30">
         <f t="shared" si="7"/>
-        <v>-505042</v>
+        <v>0</v>
       </c>
       <c r="AH13" s="30">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>1599490.0876514099</v>
       </c>
     </row>
     <row r="14" spans="1:34" x14ac:dyDescent="0.3">
-      <c r="A14" s="32">
+      <c r="A14" s="31">
         <v>0.266897</v>
       </c>
       <c r="B14" s="26">
         <v>43200</v>
       </c>
-      <c r="C14" s="26">
-        <v>0</v>
-      </c>
-      <c r="D14" s="26">
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14">
         <v>1358200</v>
       </c>
-      <c r="E14" s="26">
-        <v>-497513</v>
-      </c>
-      <c r="F14" s="26">
-        <v>0</v>
-      </c>
-      <c r="G14" s="26">
-        <v>0</v>
-      </c>
-      <c r="H14" s="26">
+      <c r="E14">
+        <v>-497512.84905450698</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+      <c r="G14">
+        <v>0</v>
+      </c>
+      <c r="H14">
         <v>1020937</v>
       </c>
-      <c r="I14" s="26">
-        <v>0</v>
-      </c>
-      <c r="J14" s="26">
-        <v>0</v>
-      </c>
-      <c r="K14" s="26">
-        <v>0</v>
-      </c>
-      <c r="L14" s="26">
-        <v>0</v>
-      </c>
-      <c r="M14" s="26">
-        <v>0</v>
-      </c>
-      <c r="N14" s="26">
+      <c r="I14">
+        <v>0</v>
+      </c>
+      <c r="J14">
+        <v>0</v>
+      </c>
+      <c r="K14">
+        <v>0</v>
+      </c>
+      <c r="L14">
+        <v>0</v>
+      </c>
+      <c r="M14">
+        <v>0</v>
+      </c>
+      <c r="N14">
         <v>-160250</v>
       </c>
-      <c r="O14" s="26">
-        <v>0</v>
-      </c>
-      <c r="P14" s="26">
-        <v>0.40910400000000002</v>
-      </c>
-      <c r="Q14" s="26">
+      <c r="O14">
+        <v>-718980.72808187502</v>
+      </c>
+      <c r="P14">
+        <v>0.40910357302679901</v>
+      </c>
+      <c r="Q14">
         <v>0.5</v>
       </c>
-      <c r="R14" s="26">
-        <v>0.10066799999999999</v>
-      </c>
-      <c r="S14" s="26">
-        <v>0.72573299999999996</v>
-      </c>
-      <c r="T14" s="26">
-        <v>1881624</v>
-      </c>
-      <c r="U14" s="26">
-        <v>-160250</v>
-      </c>
-      <c r="V14" s="26">
-        <v>0.17035500000000001</v>
-      </c>
-      <c r="W14" s="26">
+      <c r="R14">
+        <v>0.10066812439261399</v>
+      </c>
+      <c r="S14">
+        <v>0.72573250802649503</v>
+      </c>
+      <c r="T14">
+        <v>1881624.15094549</v>
+      </c>
+      <c r="U14">
+        <v>-879230.72808187502</v>
+      </c>
+      <c r="V14">
+        <v>0.17035473900000001</v>
+      </c>
+      <c r="W14">
         <v>0.12872</v>
       </c>
       <c r="X14" s="28">
@@ -4127,11 +4116,11 @@
       </c>
       <c r="Y14" s="28">
         <f t="shared" si="1"/>
-        <v>1881624</v>
+        <v>1881624.15094549</v>
       </c>
       <c r="Z14" s="28">
         <f t="shared" si="2"/>
-        <v>-160250</v>
+        <v>-879230.72808187502</v>
       </c>
       <c r="AA14" s="28">
         <f t="shared" si="3"/>
@@ -4139,7 +4128,7 @@
       </c>
       <c r="AB14" s="30">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>3.0267983675003052E-9</v>
       </c>
       <c r="AC14" s="30">
         <f t="shared" si="5"/>
@@ -4147,7 +4136,7 @@
       </c>
       <c r="AD14" s="30">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>3.0267983675003052E-9</v>
       </c>
       <c r="AE14" s="30">
         <f>IF('Day1'!A14&lt;KPI!$B$15,1,0)</f>
@@ -4159,7 +4148,7 @@
       </c>
       <c r="AG14" s="30">
         <f t="shared" si="7"/>
-        <v>-497513</v>
+        <v>0</v>
       </c>
       <c r="AH14" s="30">
         <f t="shared" si="8"/>
@@ -4167,73 +4156,73 @@
       </c>
     </row>
     <row r="15" spans="1:34" x14ac:dyDescent="0.3">
-      <c r="A15" s="32">
+      <c r="A15" s="31">
         <v>0.26474700000000001</v>
       </c>
       <c r="B15" s="26">
         <v>46800</v>
       </c>
-      <c r="C15" s="26">
-        <v>0</v>
-      </c>
-      <c r="D15" s="26">
-        <v>931306.3</v>
-      </c>
-      <c r="E15" s="26">
-        <v>-507461</v>
-      </c>
-      <c r="F15" s="26">
-        <v>0</v>
-      </c>
-      <c r="G15" s="26">
-        <v>0</v>
-      </c>
-      <c r="H15" s="26">
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <v>931306.25</v>
+      </c>
+      <c r="E15">
+        <v>-507461.41817917099</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+      <c r="G15">
+        <v>0</v>
+      </c>
+      <c r="H15">
         <v>583952</v>
       </c>
-      <c r="I15" s="26">
-        <v>0</v>
-      </c>
-      <c r="J15" s="26">
-        <v>0</v>
-      </c>
-      <c r="K15" s="26">
-        <v>0</v>
-      </c>
-      <c r="L15" s="26">
-        <v>0</v>
-      </c>
-      <c r="M15" s="26">
-        <v>0</v>
-      </c>
-      <c r="N15" s="26">
-        <v>-160108</v>
-      </c>
-      <c r="O15" s="26">
-        <v>-1317.15</v>
-      </c>
-      <c r="P15" s="26">
-        <v>0.25906400000000002</v>
-      </c>
-      <c r="Q15" s="26">
+      <c r="I15">
+        <v>0</v>
+      </c>
+      <c r="J15">
+        <v>0</v>
+      </c>
+      <c r="K15">
+        <v>0</v>
+      </c>
+      <c r="L15">
+        <v>0</v>
+      </c>
+      <c r="M15">
+        <v>0</v>
+      </c>
+      <c r="N15">
+        <v>-160107.5</v>
+      </c>
+      <c r="O15">
+        <v>-719568.8823518462</v>
+      </c>
+      <c r="P15">
+        <v>0.259063872264779</v>
+      </c>
+      <c r="Q15">
         <v>0.5</v>
       </c>
-      <c r="R15" s="26">
-        <v>0.10066799999999999</v>
-      </c>
-      <c r="S15" s="26">
-        <v>0.764324</v>
-      </c>
-      <c r="T15" s="26">
-        <v>1007797</v>
-      </c>
-      <c r="U15" s="26">
-        <v>-161425</v>
-      </c>
-      <c r="V15" s="26">
-        <v>0.171295</v>
-      </c>
-      <c r="W15" s="26">
+      <c r="R15">
+        <v>0.10066812439261399</v>
+      </c>
+      <c r="S15">
+        <v>0.764324159507901</v>
+      </c>
+      <c r="T15">
+        <v>1007796.83182083</v>
+      </c>
+      <c r="U15">
+        <v>-879676.38235184795</v>
+      </c>
+      <c r="V15">
+        <v>0.171294636</v>
+      </c>
+      <c r="W15">
         <v>0.12992999999999999</v>
       </c>
       <c r="X15" s="28">
@@ -4242,11 +4231,11 @@
       </c>
       <c r="Y15" s="28">
         <f t="shared" si="1"/>
-        <v>1007797</v>
+        <v>1007796.83182083</v>
       </c>
       <c r="Z15" s="28">
         <f t="shared" si="2"/>
-        <v>-161425</v>
+        <v>-879676.38235184795</v>
       </c>
       <c r="AA15" s="28">
         <f t="shared" si="3"/>
@@ -4254,15 +4243,15 @@
       </c>
       <c r="AB15" s="30">
         <f t="shared" si="4"/>
-        <v>0.30000000004656613</v>
+        <v>-9.3132257461547852E-10</v>
       </c>
       <c r="AC15" s="30">
         <f t="shared" si="5"/>
-        <v>-0.14999999999417923</v>
+        <v>1.7462298274040222E-9</v>
       </c>
       <c r="AD15" s="30">
         <f t="shared" si="6"/>
-        <v>0.15000000002328306</v>
+        <v>8.149072527885437E-10</v>
       </c>
       <c r="AE15" s="30">
         <f>IF('Day1'!A15&lt;KPI!$B$15,1,0)</f>
@@ -4274,81 +4263,81 @@
       </c>
       <c r="AG15" s="30">
         <f t="shared" si="7"/>
-        <v>-507461</v>
+        <v>0</v>
       </c>
       <c r="AH15" s="30">
         <f t="shared" si="8"/>
-        <v>-1317.15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:34" x14ac:dyDescent="0.3">
-      <c r="A16" s="32">
+      <c r="A16" s="31">
         <v>0.26649400000000001</v>
       </c>
       <c r="B16" s="26">
         <v>50400</v>
       </c>
-      <c r="C16" s="26">
-        <v>0</v>
-      </c>
-      <c r="D16" s="26">
-        <v>1449738</v>
-      </c>
-      <c r="E16" s="26">
-        <v>-539057</v>
-      </c>
-      <c r="F16" s="26">
-        <v>0</v>
-      </c>
-      <c r="G16" s="26">
-        <v>0</v>
-      </c>
-      <c r="H16" s="26">
+      <c r="C16">
+        <v>0</v>
+      </c>
+      <c r="D16">
+        <v>1449737.5</v>
+      </c>
+      <c r="E16">
+        <v>-539057.18036732206</v>
+      </c>
+      <c r="F16">
+        <v>0</v>
+      </c>
+      <c r="G16">
+        <v>0</v>
+      </c>
+      <c r="H16">
         <v>1077080</v>
       </c>
-      <c r="I16" s="26">
-        <v>0</v>
-      </c>
-      <c r="J16" s="26">
-        <v>0</v>
-      </c>
-      <c r="K16" s="26">
-        <v>0</v>
-      </c>
-      <c r="L16" s="26">
-        <v>0</v>
-      </c>
-      <c r="M16" s="26">
-        <v>0</v>
-      </c>
-      <c r="N16" s="26">
+      <c r="I16">
+        <v>0</v>
+      </c>
+      <c r="J16">
+        <v>0</v>
+      </c>
+      <c r="K16">
+        <v>0</v>
+      </c>
+      <c r="L16">
+        <v>0</v>
+      </c>
+      <c r="M16">
+        <v>0</v>
+      </c>
+      <c r="N16">
         <v>-166400</v>
       </c>
-      <c r="O16" s="26">
-        <v>-1317.15</v>
-      </c>
-      <c r="P16" s="26">
-        <v>0.17180400000000001</v>
-      </c>
-      <c r="Q16" s="26">
+      <c r="O16">
+        <v>-694402.21568518016</v>
+      </c>
+      <c r="P16">
+        <v>0.17180429104536099</v>
+      </c>
+      <c r="Q16">
         <v>0.5</v>
       </c>
-      <c r="R16" s="26">
-        <v>0.10066799999999999</v>
-      </c>
-      <c r="S16" s="26">
-        <v>0.80443299999999995</v>
-      </c>
-      <c r="T16" s="26">
-        <v>1987760</v>
-      </c>
-      <c r="U16" s="26">
-        <v>-167717</v>
-      </c>
-      <c r="V16" s="26">
-        <v>0.17043700000000001</v>
-      </c>
-      <c r="W16" s="26">
+      <c r="R16">
+        <v>0.10066812439261399</v>
+      </c>
+      <c r="S16">
+        <v>0.80443252923765196</v>
+      </c>
+      <c r="T16">
+        <v>1987760.3196326799</v>
+      </c>
+      <c r="U16">
+        <v>-860802.21568518097</v>
+      </c>
+      <c r="V16">
+        <v>0.170437012</v>
+      </c>
+      <c r="W16">
         <v>0.12889999999999999</v>
       </c>
       <c r="X16" s="28">
@@ -4357,11 +4346,11 @@
       </c>
       <c r="Y16" s="28">
         <f t="shared" si="1"/>
-        <v>1987760</v>
+        <v>1987760.3196326799</v>
       </c>
       <c r="Z16" s="28">
         <f t="shared" si="2"/>
-        <v>-167717</v>
+        <v>-860802.21568518097</v>
       </c>
       <c r="AA16" s="28">
         <f t="shared" si="3"/>
@@ -4369,15 +4358,15 @@
       </c>
       <c r="AB16" s="30">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>-2.0954757928848267E-9</v>
       </c>
       <c r="AC16" s="30">
         <f t="shared" si="5"/>
-        <v>-0.14999999999417923</v>
+        <v>0</v>
       </c>
       <c r="AD16" s="30">
         <f t="shared" si="6"/>
-        <v>0.85000000009313226</v>
+        <v>-1.280568540096283E-9</v>
       </c>
       <c r="AE16" s="30">
         <f>IF('Day1'!A16&lt;KPI!$B$15,1,0)</f>
@@ -4389,81 +4378,81 @@
       </c>
       <c r="AG16" s="30">
         <f t="shared" si="7"/>
-        <v>-539057</v>
+        <v>0</v>
       </c>
       <c r="AH16" s="30">
         <f t="shared" si="8"/>
-        <v>-1317.15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:34" x14ac:dyDescent="0.3">
-      <c r="A17" s="32">
+      <c r="A17" s="31">
         <v>0.270067</v>
       </c>
       <c r="B17" s="26">
         <v>54000</v>
       </c>
-      <c r="C17" s="26">
-        <v>0</v>
-      </c>
-      <c r="D17" s="26">
+      <c r="C17">
+        <v>0</v>
+      </c>
+      <c r="D17">
         <v>1487075</v>
       </c>
-      <c r="E17" s="26">
-        <v>-556815</v>
-      </c>
-      <c r="F17" s="26">
-        <v>0</v>
-      </c>
-      <c r="G17" s="26">
-        <v>0</v>
-      </c>
-      <c r="H17" s="26">
-        <v>389354</v>
-      </c>
-      <c r="I17" s="26">
-        <v>0</v>
-      </c>
-      <c r="J17" s="26">
-        <v>0</v>
-      </c>
-      <c r="K17" s="26">
-        <v>0</v>
-      </c>
-      <c r="L17" s="26">
-        <v>0</v>
-      </c>
-      <c r="M17" s="26">
-        <v>0</v>
-      </c>
-      <c r="N17" s="26">
+      <c r="E17">
+        <v>-556814.99787919899</v>
+      </c>
+      <c r="F17">
+        <v>0</v>
+      </c>
+      <c r="G17">
+        <v>0</v>
+      </c>
+      <c r="H17">
+        <v>389354.02318466298</v>
+      </c>
+      <c r="I17">
+        <v>0</v>
+      </c>
+      <c r="J17">
+        <v>0</v>
+      </c>
+      <c r="K17">
+        <v>0</v>
+      </c>
+      <c r="L17">
+        <v>0</v>
+      </c>
+      <c r="M17">
+        <v>0</v>
+      </c>
+      <c r="N17">
         <v>-159900</v>
       </c>
-      <c r="O17" s="26">
-        <v>-2634.3</v>
-      </c>
-      <c r="P17" s="26">
-        <v>5.6777000000000001E-2</v>
-      </c>
-      <c r="Q17" s="26">
+      <c r="O17">
+        <v>-720157.03662181948</v>
+      </c>
+      <c r="P17">
+        <v>5.6777481845124898E-2</v>
+      </c>
+      <c r="Q17">
         <v>0.5</v>
       </c>
-      <c r="R17" s="26">
-        <v>0.10066799999999999</v>
-      </c>
-      <c r="S17" s="26">
-        <v>0.842974</v>
-      </c>
-      <c r="T17" s="26">
-        <v>1319614</v>
-      </c>
-      <c r="U17" s="26">
-        <v>-162534</v>
-      </c>
-      <c r="V17" s="26">
-        <v>0.16783999999999999</v>
-      </c>
-      <c r="W17" s="26">
+      <c r="R17">
+        <v>0.10066812439261399</v>
+      </c>
+      <c r="S17">
+        <v>0.84297416577483397</v>
+      </c>
+      <c r="T17">
+        <v>1319614.02530546</v>
+      </c>
+      <c r="U17">
+        <v>-880057.03662181995</v>
+      </c>
+      <c r="V17">
+        <v>0.167840183</v>
+      </c>
+      <c r="W17">
         <v>0.12529000000000001</v>
       </c>
       <c r="X17" s="28">
@@ -4472,11 +4461,11 @@
       </c>
       <c r="Y17" s="28">
         <f t="shared" si="1"/>
-        <v>1319614</v>
+        <v>1319614.02530546</v>
       </c>
       <c r="Z17" s="28">
         <f t="shared" si="2"/>
-        <v>-162534</v>
+        <v>-880057.03662181995</v>
       </c>
       <c r="AA17" s="28">
         <f t="shared" si="3"/>
@@ -4484,15 +4473,15 @@
       </c>
       <c r="AB17" s="30">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>3.9581209421157837E-9</v>
       </c>
       <c r="AC17" s="30">
         <f t="shared" si="5"/>
-        <v>-0.29999999998835847</v>
+        <v>0</v>
       </c>
       <c r="AD17" s="30">
         <f t="shared" si="6"/>
-        <v>-0.30000000004656613</v>
+        <v>4.4237822294235229E-9</v>
       </c>
       <c r="AE17" s="30">
         <f>IF('Day1'!A17&lt;KPI!$B$15,1,0)</f>
@@ -4504,81 +4493,81 @@
       </c>
       <c r="AG17" s="30">
         <f t="shared" si="7"/>
-        <v>-556815</v>
+        <v>0</v>
       </c>
       <c r="AH17" s="30">
         <f t="shared" si="8"/>
-        <v>-2634.3</v>
+        <v>1319614.02530546</v>
       </c>
     </row>
     <row r="18" spans="1:34" x14ac:dyDescent="0.3">
-      <c r="A18" s="32">
+      <c r="A18" s="31">
         <v>0.27431899999999998</v>
       </c>
       <c r="B18" s="26">
         <v>57600</v>
       </c>
-      <c r="C18" s="26">
-        <v>0</v>
-      </c>
-      <c r="D18" s="26">
-        <v>1547713</v>
-      </c>
-      <c r="E18" s="26">
-        <v>-548009</v>
-      </c>
-      <c r="F18" s="26">
-        <v>0</v>
-      </c>
-      <c r="G18" s="26">
-        <v>0</v>
-      </c>
-      <c r="H18" s="26">
-        <v>0</v>
-      </c>
-      <c r="I18" s="26">
-        <v>0</v>
-      </c>
-      <c r="J18" s="26">
-        <v>0</v>
-      </c>
-      <c r="K18" s="26">
-        <v>0</v>
-      </c>
-      <c r="L18" s="26">
-        <v>0</v>
-      </c>
-      <c r="M18" s="26">
-        <v>0</v>
-      </c>
-      <c r="N18" s="26">
+      <c r="C18">
+        <v>0</v>
+      </c>
+      <c r="D18">
+        <v>1547712.5</v>
+      </c>
+      <c r="E18">
+        <v>-548009.32167300896</v>
+      </c>
+      <c r="F18">
+        <v>0</v>
+      </c>
+      <c r="G18">
+        <v>0</v>
+      </c>
+      <c r="H18">
+        <v>0</v>
+      </c>
+      <c r="I18">
+        <v>0</v>
+      </c>
+      <c r="J18">
+        <v>0</v>
+      </c>
+      <c r="K18">
+        <v>0</v>
+      </c>
+      <c r="L18">
+        <v>0</v>
+      </c>
+      <c r="M18">
+        <v>0</v>
+      </c>
+      <c r="N18">
         <v>-148700</v>
       </c>
-      <c r="O18" s="26">
-        <v>-2634.3</v>
-      </c>
-      <c r="P18" s="26">
-        <v>1.7139000000000001E-2</v>
-      </c>
-      <c r="Q18" s="26">
+      <c r="O18">
+        <v>-765235.41167452745</v>
+      </c>
+      <c r="P18">
+        <v>1.7139204634447399E-2</v>
+      </c>
+      <c r="Q18">
         <v>0.5</v>
       </c>
-      <c r="R18" s="26">
-        <v>0.10066799999999999</v>
-      </c>
-      <c r="S18" s="26">
-        <v>0.87881600000000004</v>
-      </c>
-      <c r="T18" s="26">
-        <v>999703.2</v>
-      </c>
-      <c r="U18" s="26">
-        <v>-151334</v>
-      </c>
-      <c r="V18" s="26">
-        <v>0.17468800000000001</v>
-      </c>
-      <c r="W18" s="26">
+      <c r="R18">
+        <v>0.10066812439261399</v>
+      </c>
+      <c r="S18">
+        <v>0.87881620050328302</v>
+      </c>
+      <c r="T18">
+        <v>999703.17832699104</v>
+      </c>
+      <c r="U18">
+        <v>-913935.41167452803</v>
+      </c>
+      <c r="V18">
+        <v>0.17468782299999999</v>
+      </c>
+      <c r="W18">
         <v>0.12831999999999999</v>
       </c>
       <c r="X18" s="28">
@@ -4587,11 +4576,11 @@
       </c>
       <c r="Y18" s="28">
         <f t="shared" si="1"/>
-        <v>999703.2</v>
+        <v>999703.17832699104</v>
       </c>
       <c r="Z18" s="28">
         <f t="shared" si="2"/>
-        <v>-151334</v>
+        <v>-913935.41167452803</v>
       </c>
       <c r="AA18" s="28">
         <f t="shared" si="3"/>
@@ -4599,15 +4588,15 @@
       </c>
       <c r="AB18" s="30">
         <f t="shared" si="4"/>
-        <v>0.80000000004656613</v>
+        <v>0</v>
       </c>
       <c r="AC18" s="30">
         <f t="shared" si="5"/>
-        <v>-0.29999999998835847</v>
+        <v>0</v>
       </c>
       <c r="AD18" s="30">
         <f t="shared" si="6"/>
-        <v>0.5</v>
+        <v>5.8207660913467407E-10</v>
       </c>
       <c r="AE18" s="30">
         <f>IF('Day1'!A18&lt;KPI!$B$15,1,0)</f>
@@ -4619,81 +4608,81 @@
       </c>
       <c r="AG18" s="30">
         <f t="shared" si="7"/>
-        <v>-548009</v>
+        <v>0</v>
       </c>
       <c r="AH18" s="30">
         <f t="shared" si="8"/>
-        <v>-2634.3</v>
+        <v>999703.17832699104</v>
       </c>
     </row>
     <row r="19" spans="1:34" x14ac:dyDescent="0.3">
-      <c r="A19" s="32">
+      <c r="A19" s="31">
         <v>0.27111299999999999</v>
       </c>
       <c r="B19" s="26">
         <v>61200</v>
       </c>
-      <c r="C19" s="26">
-        <v>0</v>
-      </c>
-      <c r="D19" s="26">
+      <c r="C19">
+        <v>0</v>
+      </c>
+      <c r="D19">
         <v>612237.5</v>
       </c>
-      <c r="E19" s="26">
-        <v>-497719</v>
-      </c>
-      <c r="F19" s="26">
-        <v>0</v>
-      </c>
-      <c r="G19" s="26">
-        <v>0</v>
-      </c>
-      <c r="H19" s="26">
-        <v>0</v>
-      </c>
-      <c r="I19" s="26">
-        <v>0</v>
-      </c>
-      <c r="J19" s="26">
-        <v>0</v>
-      </c>
-      <c r="K19" s="26">
-        <v>0</v>
-      </c>
-      <c r="L19" s="26">
-        <v>0</v>
-      </c>
-      <c r="M19" s="26">
-        <v>0</v>
-      </c>
-      <c r="N19" s="26">
+      <c r="E19">
+        <v>-497718.72584464902</v>
+      </c>
+      <c r="F19">
+        <v>0</v>
+      </c>
+      <c r="G19">
+        <v>0</v>
+      </c>
+      <c r="H19">
+        <v>0</v>
+      </c>
+      <c r="I19">
+        <v>0</v>
+      </c>
+      <c r="J19">
+        <v>0</v>
+      </c>
+      <c r="K19">
+        <v>0</v>
+      </c>
+      <c r="L19">
+        <v>0</v>
+      </c>
+      <c r="M19">
+        <v>0</v>
+      </c>
+      <c r="N19">
         <v>-153700</v>
       </c>
-      <c r="O19" s="26">
-        <v>-2634.3</v>
-      </c>
-      <c r="P19" s="26">
-        <v>1.7139000000000001E-2</v>
-      </c>
-      <c r="Q19" s="26">
+      <c r="O19">
+        <v>-745323.70328848646</v>
+      </c>
+      <c r="P19">
+        <v>1.7139204634447399E-2</v>
+      </c>
+      <c r="Q19">
         <v>0.5</v>
       </c>
-      <c r="R19" s="26">
-        <v>0.10066799999999999</v>
-      </c>
-      <c r="S19" s="26">
-        <v>0.91586299999999998</v>
-      </c>
-      <c r="T19" s="26">
-        <v>114518.8</v>
-      </c>
-      <c r="U19" s="26">
-        <v>-156334</v>
-      </c>
-      <c r="V19" s="26">
-        <v>0.18501300000000001</v>
-      </c>
-      <c r="W19" s="26">
+      <c r="R19">
+        <v>0.10066812439261399</v>
+      </c>
+      <c r="S19">
+        <v>0.91586341461063103</v>
+      </c>
+      <c r="T19">
+        <v>114518.774155351</v>
+      </c>
+      <c r="U19">
+        <v>-899023.70328848599</v>
+      </c>
+      <c r="V19">
+        <v>0.185012962</v>
+      </c>
+      <c r="W19">
         <v>0.13632</v>
       </c>
       <c r="X19" s="28">
@@ -4702,11 +4691,11 @@
       </c>
       <c r="Y19" s="28">
         <f t="shared" si="1"/>
-        <v>114518.8</v>
+        <v>114518.774155351</v>
       </c>
       <c r="Z19" s="28">
         <f t="shared" si="2"/>
-        <v>-156334</v>
+        <v>-899023.70328848599</v>
       </c>
       <c r="AA19" s="28">
         <f t="shared" si="3"/>
@@ -4714,15 +4703,15 @@
       </c>
       <c r="AB19" s="30">
         <f t="shared" si="4"/>
-        <v>-0.30000000000291038</v>
+        <v>0</v>
       </c>
       <c r="AC19" s="30">
         <f t="shared" si="5"/>
-        <v>-0.29999999998835847</v>
+        <v>0</v>
       </c>
       <c r="AD19" s="30">
         <f t="shared" si="6"/>
-        <v>-0.60000000000582077</v>
+        <v>-4.6566128730773926E-10</v>
       </c>
       <c r="AE19" s="30">
         <f>IF('Day1'!A19&lt;KPI!$B$15,1,0)</f>
@@ -4734,86 +4723,86 @@
       </c>
       <c r="AG19" s="30">
         <f t="shared" si="7"/>
-        <v>-497719</v>
+        <v>0</v>
       </c>
       <c r="AH19" s="30">
         <f t="shared" si="8"/>
-        <v>-2634.3</v>
+        <v>114518.774155351</v>
       </c>
     </row>
     <row r="20" spans="1:34" x14ac:dyDescent="0.3">
-      <c r="A20" s="32">
+      <c r="A20" s="31">
         <v>0.28212799999999999</v>
       </c>
       <c r="B20" s="26">
         <v>64800</v>
       </c>
-      <c r="C20" s="26">
-        <v>0</v>
-      </c>
-      <c r="D20" s="26">
+      <c r="C20">
+        <v>0</v>
+      </c>
+      <c r="D20">
         <v>79631.25</v>
       </c>
-      <c r="E20" s="26">
-        <v>-417148</v>
-      </c>
-      <c r="F20" s="26">
-        <v>0</v>
-      </c>
-      <c r="G20" s="26">
-        <v>0</v>
-      </c>
-      <c r="H20" s="26">
+      <c r="E20">
+        <v>-417148.00624470599</v>
+      </c>
+      <c r="F20">
+        <v>0</v>
+      </c>
+      <c r="G20">
+        <v>0</v>
+      </c>
+      <c r="H20">
         <v>-683000</v>
       </c>
-      <c r="I20" s="26">
-        <v>0</v>
-      </c>
-      <c r="J20" s="26">
+      <c r="I20">
+        <v>0</v>
+      </c>
+      <c r="J20">
         <v>-337516</v>
       </c>
-      <c r="K20" s="26">
-        <v>0</v>
-      </c>
-      <c r="L20" s="26">
-        <v>0</v>
-      </c>
-      <c r="M20" s="26">
-        <v>0</v>
-      </c>
-      <c r="N20" s="26">
+      <c r="K20">
+        <v>0</v>
+      </c>
+      <c r="L20">
+        <v>0</v>
+      </c>
+      <c r="M20">
+        <v>0</v>
+      </c>
+      <c r="N20">
         <v>-216000</v>
       </c>
-      <c r="O20" s="26">
-        <v>-10537.2</v>
-      </c>
-      <c r="P20" s="26">
-        <v>1.7139000000000001E-2</v>
-      </c>
-      <c r="Q20" s="26">
+      <c r="O20">
+        <v>-475871.90082644694</v>
+      </c>
+      <c r="P20">
+        <v>1.7139204634447399E-2</v>
+      </c>
+      <c r="Q20">
         <v>0.5</v>
       </c>
-      <c r="R20" s="26">
-        <v>0.14330899999999999</v>
-      </c>
-      <c r="S20" s="26">
-        <v>0.96792699999999998</v>
-      </c>
-      <c r="T20" s="26">
-        <v>-1358033</v>
-      </c>
-      <c r="U20" s="26">
-        <v>-226537</v>
-      </c>
-      <c r="V20" s="26">
-        <v>0.25895099999999999</v>
-      </c>
-      <c r="W20" s="26">
+      <c r="R20">
+        <v>0.14330862973760899</v>
+      </c>
+      <c r="S20">
+        <v>0.96792716377905696</v>
+      </c>
+      <c r="T20">
+        <v>-1358032.7562447099</v>
+      </c>
+      <c r="U20">
+        <v>-691871.90082644694</v>
+      </c>
+      <c r="V20">
+        <v>0.25895084000000002</v>
+      </c>
+      <c r="W20">
         <v>0.19972000000000001</v>
       </c>
       <c r="X20" s="28">
         <f t="shared" si="0"/>
-        <v>-1358033</v>
+        <v>-1358032.7562447099</v>
       </c>
       <c r="Y20" s="28">
         <f t="shared" si="1"/>
@@ -4821,7 +4810,7 @@
       </c>
       <c r="Z20" s="28">
         <f t="shared" si="2"/>
-        <v>-226537</v>
+        <v>-691871.90082644694</v>
       </c>
       <c r="AA20" s="28">
         <f t="shared" si="3"/>
@@ -4829,15 +4818,15 @@
       </c>
       <c r="AB20" s="30">
         <f t="shared" si="4"/>
-        <v>0.25</v>
+        <v>3.9581209421157837E-9</v>
       </c>
       <c r="AC20" s="30">
         <f t="shared" si="5"/>
-        <v>-0.20000000001164153</v>
+        <v>0</v>
       </c>
       <c r="AD20" s="30">
         <f t="shared" si="6"/>
-        <v>5.0000000046566129E-2</v>
+        <v>3.9581209421157837E-9</v>
       </c>
       <c r="AE20" s="30">
         <f>IF('Day1'!A20&lt;KPI!$B$15,1,0)</f>
@@ -4849,86 +4838,86 @@
       </c>
       <c r="AG20" s="30">
         <f t="shared" si="7"/>
-        <v>-417148</v>
+        <v>0</v>
       </c>
       <c r="AH20" s="30">
         <f t="shared" si="8"/>
-        <v>-10537.2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:34" x14ac:dyDescent="0.3">
-      <c r="A21" s="32">
+      <c r="A21" s="31">
         <v>0.28089700000000001</v>
       </c>
       <c r="B21" s="26">
         <v>68400</v>
       </c>
-      <c r="C21" s="26">
-        <v>0</v>
-      </c>
-      <c r="D21" s="26">
+      <c r="C21">
+        <v>0</v>
+      </c>
+      <c r="D21">
         <v>31.25</v>
       </c>
-      <c r="E21" s="26">
-        <v>-465631</v>
-      </c>
-      <c r="F21" s="26">
-        <v>0</v>
-      </c>
-      <c r="G21" s="26">
-        <v>0</v>
-      </c>
-      <c r="H21" s="26">
+      <c r="E21">
+        <v>-465631.27859207703</v>
+      </c>
+      <c r="F21">
+        <v>0</v>
+      </c>
+      <c r="G21">
+        <v>0</v>
+      </c>
+      <c r="H21">
         <v>-465600</v>
       </c>
-      <c r="I21" s="26">
-        <v>0</v>
-      </c>
-      <c r="J21" s="26">
+      <c r="I21">
+        <v>0</v>
+      </c>
+      <c r="J21">
         <v>-337500</v>
       </c>
-      <c r="K21" s="26">
-        <v>0</v>
-      </c>
-      <c r="L21" s="26">
-        <v>0</v>
-      </c>
-      <c r="M21" s="26">
-        <v>0</v>
-      </c>
-      <c r="N21" s="26">
-        <v>0</v>
-      </c>
-      <c r="O21" s="26">
-        <v>-10537.2</v>
-      </c>
-      <c r="P21" s="26">
-        <v>0.13763800000000001</v>
-      </c>
-      <c r="Q21" s="26">
+      <c r="K21">
+        <v>0</v>
+      </c>
+      <c r="L21">
+        <v>0</v>
+      </c>
+      <c r="M21">
+        <v>0</v>
+      </c>
+      <c r="N21">
+        <v>0</v>
+      </c>
+      <c r="O21">
+        <v>-601455.23415977997</v>
+      </c>
+      <c r="P21">
+        <v>0.13763809437916499</v>
+      </c>
+      <c r="Q21">
         <v>0.5</v>
       </c>
-      <c r="R21" s="26">
-        <v>0.22858800000000001</v>
-      </c>
-      <c r="S21" s="26">
+      <c r="R21">
+        <v>0.22858761904761901</v>
+      </c>
+      <c r="S21">
         <v>1</v>
       </c>
-      <c r="T21" s="26">
-        <v>-1268700</v>
-      </c>
-      <c r="U21" s="26">
-        <v>-10537.2</v>
-      </c>
-      <c r="V21" s="26">
-        <v>0.27743400000000001</v>
-      </c>
-      <c r="W21" s="26">
+      <c r="T21">
+        <v>-1268700.0285920801</v>
+      </c>
+      <c r="U21">
+        <v>-601455.23415977997</v>
+      </c>
+      <c r="V21">
+        <v>0.27743423</v>
+      </c>
+      <c r="W21">
         <v>0.21782000000000001</v>
       </c>
       <c r="X21" s="28">
         <f t="shared" si="0"/>
-        <v>-1268700</v>
+        <v>-1268700.0285920801</v>
       </c>
       <c r="Y21" s="28">
         <f t="shared" si="1"/>
@@ -4936,7 +4925,7 @@
       </c>
       <c r="Z21" s="28">
         <f t="shared" si="2"/>
-        <v>-10537.2</v>
+        <v>-601455.23415977997</v>
       </c>
       <c r="AA21" s="28">
         <f t="shared" si="3"/>
@@ -4944,7 +4933,7 @@
       </c>
       <c r="AB21" s="30">
         <f t="shared" si="4"/>
-        <v>0.25</v>
+        <v>3.0267983675003052E-9</v>
       </c>
       <c r="AC21" s="30">
         <f t="shared" si="5"/>
@@ -4952,7 +4941,7 @@
       </c>
       <c r="AD21" s="30">
         <f t="shared" si="6"/>
-        <v>0.25000000004729372</v>
+        <v>3.0267983675003052E-9</v>
       </c>
       <c r="AE21" s="30">
         <f>IF('Day1'!A21&lt;KPI!$B$15,1,0)</f>
@@ -4964,86 +4953,86 @@
       </c>
       <c r="AG21" s="30">
         <f t="shared" si="7"/>
-        <v>-465631</v>
+        <v>0</v>
       </c>
       <c r="AH21" s="30">
         <f t="shared" si="8"/>
-        <v>-10537.2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:34" x14ac:dyDescent="0.3">
-      <c r="A22" s="32">
+      <c r="A22" s="31">
         <v>0.27615600000000001</v>
       </c>
       <c r="B22" s="26">
         <v>72000</v>
       </c>
-      <c r="C22" s="26">
-        <v>0</v>
-      </c>
-      <c r="D22" s="26">
-        <v>0</v>
-      </c>
-      <c r="E22" s="26">
+      <c r="C22">
+        <v>0</v>
+      </c>
+      <c r="D22">
+        <v>0</v>
+      </c>
+      <c r="E22">
+        <v>-512742.02974724898</v>
+      </c>
+      <c r="F22">
+        <v>0</v>
+      </c>
+      <c r="G22">
+        <v>0</v>
+      </c>
+      <c r="H22">
         <v>-512742</v>
       </c>
-      <c r="F22" s="26">
-        <v>0</v>
-      </c>
-      <c r="G22" s="26">
-        <v>0</v>
-      </c>
-      <c r="H22" s="26">
-        <v>-512742</v>
-      </c>
-      <c r="I22" s="26">
-        <v>0</v>
-      </c>
-      <c r="J22" s="26">
+      <c r="I22">
+        <v>0</v>
+      </c>
+      <c r="J22">
         <v>-337500</v>
       </c>
-      <c r="K22" s="26">
-        <v>0</v>
-      </c>
-      <c r="L22" s="26">
-        <v>0</v>
-      </c>
-      <c r="M22" s="26">
-        <v>0</v>
-      </c>
-      <c r="N22" s="26">
-        <v>0</v>
-      </c>
-      <c r="O22" s="26">
-        <v>-2634.3</v>
-      </c>
-      <c r="P22" s="26">
-        <v>0.21990299999999999</v>
-      </c>
-      <c r="Q22" s="26">
+      <c r="K22">
+        <v>0</v>
+      </c>
+      <c r="L22">
+        <v>0</v>
+      </c>
+      <c r="M22">
+        <v>0</v>
+      </c>
+      <c r="N22">
+        <v>0</v>
+      </c>
+      <c r="O22">
+        <v>-491009.64187327842</v>
+      </c>
+      <c r="P22">
+        <v>0.219903009430546</v>
+      </c>
+      <c r="Q22">
         <v>0.5</v>
       </c>
-      <c r="R22" s="26">
-        <v>0.31386500000000001</v>
-      </c>
-      <c r="S22" s="26">
+      <c r="R22">
+        <v>0.31386458697764802</v>
+      </c>
+      <c r="S22">
         <v>1</v>
       </c>
-      <c r="T22" s="26">
-        <v>-1362984</v>
-      </c>
-      <c r="U22" s="26">
-        <v>-2634.3</v>
-      </c>
-      <c r="V22" s="26">
-        <v>0.28452899999999998</v>
-      </c>
-      <c r="W22" s="26">
+      <c r="T22">
+        <v>-1362984.02974725</v>
+      </c>
+      <c r="U22">
+        <v>-491009.64187327801</v>
+      </c>
+      <c r="V22">
+        <v>0.28452875100000002</v>
+      </c>
+      <c r="W22">
         <v>0.22478999999999999</v>
       </c>
       <c r="X22" s="28">
         <f t="shared" si="0"/>
-        <v>-1362984</v>
+        <v>-1362984.02974725</v>
       </c>
       <c r="Y22" s="28">
         <f t="shared" si="1"/>
@@ -5051,7 +5040,7 @@
       </c>
       <c r="Z22" s="28">
         <f t="shared" si="2"/>
-        <v>-2634.3</v>
+        <v>-491009.64187327801</v>
       </c>
       <c r="AA22" s="28">
         <f t="shared" si="3"/>
@@ -5067,7 +5056,7 @@
       </c>
       <c r="AD22" s="30">
         <f t="shared" si="6"/>
-        <v>-4.638422979041934E-11</v>
+        <v>5.2386894822120667E-10</v>
       </c>
       <c r="AE22" s="30">
         <f>IF('Day1'!A22&lt;KPI!$B$15,1,0)</f>
@@ -5079,86 +5068,86 @@
       </c>
       <c r="AG22" s="30">
         <f t="shared" si="7"/>
-        <v>-512742</v>
+        <v>0</v>
       </c>
       <c r="AH22" s="30">
         <f t="shared" si="8"/>
-        <v>-2634.3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:34" x14ac:dyDescent="0.3">
-      <c r="A23" s="32">
+      <c r="A23" s="31">
         <v>0.27117200000000002</v>
       </c>
       <c r="B23" s="26">
         <v>75600</v>
       </c>
-      <c r="C23" s="26">
-        <v>0</v>
-      </c>
-      <c r="D23" s="26">
-        <v>0</v>
-      </c>
-      <c r="E23" s="26">
+      <c r="C23">
+        <v>0</v>
+      </c>
+      <c r="D23">
+        <v>0</v>
+      </c>
+      <c r="E23">
+        <v>-508746.04423543898</v>
+      </c>
+      <c r="F23">
+        <v>0</v>
+      </c>
+      <c r="G23">
+        <v>0</v>
+      </c>
+      <c r="H23">
         <v>-508746</v>
       </c>
-      <c r="F23" s="26">
-        <v>0</v>
-      </c>
-      <c r="G23" s="26">
-        <v>0</v>
-      </c>
-      <c r="H23" s="26">
-        <v>-508746</v>
-      </c>
-      <c r="I23" s="26">
-        <v>0</v>
-      </c>
-      <c r="J23" s="26">
+      <c r="I23">
+        <v>0</v>
+      </c>
+      <c r="J23">
         <v>-337500</v>
       </c>
-      <c r="K23" s="26">
-        <v>0</v>
-      </c>
-      <c r="L23" s="26">
-        <v>0</v>
-      </c>
-      <c r="M23" s="26">
-        <v>0</v>
-      </c>
-      <c r="N23" s="26">
-        <v>0</v>
-      </c>
-      <c r="O23" s="26">
-        <v>-2634.3</v>
-      </c>
-      <c r="P23" s="26">
-        <v>0.30016799999999999</v>
-      </c>
-      <c r="Q23" s="26">
+      <c r="K23">
+        <v>0</v>
+      </c>
+      <c r="L23">
+        <v>0</v>
+      </c>
+      <c r="M23">
+        <v>0</v>
+      </c>
+      <c r="N23">
+        <v>0</v>
+      </c>
+      <c r="O23">
+        <v>-296342.97520661145</v>
+      </c>
+      <c r="P23">
+        <v>0.30016808809220902</v>
+      </c>
+      <c r="Q23">
         <v>0.5</v>
       </c>
-      <c r="R23" s="26">
-        <v>0.399142</v>
-      </c>
-      <c r="S23" s="26">
+      <c r="R23">
+        <v>0.399141554907677</v>
+      </c>
+      <c r="S23">
         <v>1</v>
       </c>
-      <c r="T23" s="26">
-        <v>-1354992</v>
-      </c>
-      <c r="U23" s="26">
-        <v>-2634.3</v>
-      </c>
-      <c r="V23" s="26">
-        <v>0.28195300000000001</v>
-      </c>
-      <c r="W23" s="26">
+      <c r="T23">
+        <v>-1354992.04423544</v>
+      </c>
+      <c r="U23">
+        <v>-296342.97520661098</v>
+      </c>
+      <c r="V23">
+        <v>0.28195294799999998</v>
+      </c>
+      <c r="W23">
         <v>0.22303000000000001</v>
       </c>
       <c r="X23" s="28">
         <f t="shared" si="0"/>
-        <v>-1354992</v>
+        <v>-1354992.04423544</v>
       </c>
       <c r="Y23" s="28">
         <f t="shared" si="1"/>
@@ -5166,7 +5155,7 @@
       </c>
       <c r="Z23" s="28">
         <f t="shared" si="2"/>
-        <v>-2634.3</v>
+        <v>-296342.97520661098</v>
       </c>
       <c r="AA23" s="28">
         <f t="shared" si="3"/>
@@ -5178,11 +5167,11 @@
       </c>
       <c r="AC23" s="30">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>-4.6566128730773926E-10</v>
       </c>
       <c r="AD23" s="30">
         <f t="shared" si="6"/>
-        <v>-4.638422979041934E-11</v>
+        <v>4.6566128730773926E-10</v>
       </c>
       <c r="AE23" s="30">
         <f>IF('Day1'!A23&lt;KPI!$B$15,1,0)</f>
@@ -5194,86 +5183,86 @@
       </c>
       <c r="AG23" s="30">
         <f t="shared" si="7"/>
-        <v>-508746</v>
+        <v>0</v>
       </c>
       <c r="AH23" s="30">
         <f t="shared" si="8"/>
-        <v>-2634.3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:34" x14ac:dyDescent="0.3">
-      <c r="A24" s="32">
+      <c r="A24" s="31">
         <v>0.26649</v>
       </c>
       <c r="B24" s="26">
         <v>79200</v>
       </c>
-      <c r="C24" s="26">
-        <v>0</v>
-      </c>
-      <c r="D24" s="26">
-        <v>0</v>
-      </c>
-      <c r="E24" s="26">
+      <c r="C24">
+        <v>0</v>
+      </c>
+      <c r="D24">
+        <v>0</v>
+      </c>
+      <c r="E24">
+        <v>-510549.19361575902</v>
+      </c>
+      <c r="F24">
+        <v>0</v>
+      </c>
+      <c r="G24">
+        <v>0</v>
+      </c>
+      <c r="H24">
         <v>-510549</v>
       </c>
-      <c r="F24" s="26">
-        <v>0</v>
-      </c>
-      <c r="G24" s="26">
-        <v>0</v>
-      </c>
-      <c r="H24" s="26">
-        <v>-510549</v>
-      </c>
-      <c r="I24" s="26">
-        <v>0</v>
-      </c>
-      <c r="J24" s="26">
+      <c r="I24">
+        <v>0</v>
+      </c>
+      <c r="J24">
         <v>-337500</v>
       </c>
-      <c r="K24" s="26">
-        <v>0</v>
-      </c>
-      <c r="L24" s="26">
-        <v>0</v>
-      </c>
-      <c r="M24" s="26">
-        <v>0</v>
-      </c>
-      <c r="N24" s="26">
-        <v>0</v>
-      </c>
-      <c r="O24" s="26">
-        <v>-2634.3</v>
-      </c>
-      <c r="P24" s="26">
-        <v>0.37848700000000002</v>
-      </c>
-      <c r="Q24" s="26">
+      <c r="K24">
+        <v>0</v>
+      </c>
+      <c r="L24">
+        <v>0</v>
+      </c>
+      <c r="M24">
+        <v>0</v>
+      </c>
+      <c r="N24">
+        <v>0</v>
+      </c>
+      <c r="O24">
+        <v>-151926.3085399447</v>
+      </c>
+      <c r="P24">
+        <v>0.37848710706539301</v>
+      </c>
+      <c r="Q24">
         <v>0.5</v>
       </c>
-      <c r="R24" s="26">
-        <v>0.48441899999999999</v>
-      </c>
-      <c r="S24" s="26">
+      <c r="R24">
+        <v>0.48441852283770698</v>
+      </c>
+      <c r="S24">
         <v>1</v>
       </c>
-      <c r="T24" s="26">
-        <v>-1358598</v>
-      </c>
-      <c r="U24" s="26">
-        <v>-2634.3</v>
-      </c>
-      <c r="V24" s="26">
-        <v>0.27047399999999999</v>
-      </c>
-      <c r="W24" s="26">
+      <c r="T24">
+        <v>-1358598.19361576</v>
+      </c>
+      <c r="U24">
+        <v>-151926.30853994499</v>
+      </c>
+      <c r="V24">
+        <v>0.27047363200000002</v>
+      </c>
+      <c r="W24">
         <v>0.21471999999999999</v>
       </c>
       <c r="X24" s="28">
         <f t="shared" si="0"/>
-        <v>-1358598</v>
+        <v>-1358598.19361576</v>
       </c>
       <c r="Y24" s="28">
         <f t="shared" si="1"/>
@@ -5281,7 +5270,7 @@
       </c>
       <c r="Z24" s="28">
         <f t="shared" si="2"/>
-        <v>-2634.3</v>
+        <v>-151926.30853994499</v>
       </c>
       <c r="AA24" s="28">
         <f t="shared" si="3"/>
@@ -5293,11 +5282,11 @@
       </c>
       <c r="AC24" s="30">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>2.9103830456733704E-10</v>
       </c>
       <c r="AD24" s="30">
         <f t="shared" si="6"/>
-        <v>-4.638422979041934E-11</v>
+        <v>1.2223608791828156E-9</v>
       </c>
       <c r="AE24" s="30">
         <f>IF('Day1'!A24&lt;KPI!$B$15,1,0)</f>
@@ -5309,86 +5298,86 @@
       </c>
       <c r="AG24" s="30">
         <f t="shared" si="7"/>
-        <v>-510549</v>
+        <v>-1358598.19361576</v>
       </c>
       <c r="AH24" s="30">
         <f t="shared" si="8"/>
-        <v>-2634.3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:34" x14ac:dyDescent="0.3">
-      <c r="A25" s="32">
+      <c r="A25" s="31">
         <v>0.26110800000000001</v>
       </c>
       <c r="B25" s="26">
         <v>82800</v>
       </c>
-      <c r="C25" s="26">
-        <v>0</v>
-      </c>
-      <c r="D25" s="26">
-        <v>0</v>
-      </c>
-      <c r="E25" s="26">
-        <v>-500701</v>
-      </c>
-      <c r="F25" s="26">
-        <v>0</v>
-      </c>
-      <c r="G25" s="26">
-        <v>0</v>
-      </c>
-      <c r="H25" s="26">
+      <c r="C25">
+        <v>0</v>
+      </c>
+      <c r="D25">
+        <v>0</v>
+      </c>
+      <c r="E25">
+        <v>-500701.48059989797</v>
+      </c>
+      <c r="F25">
+        <v>0</v>
+      </c>
+      <c r="G25">
+        <v>0</v>
+      </c>
+      <c r="H25">
         <v>-725363</v>
       </c>
-      <c r="I25" s="26">
-        <v>0</v>
-      </c>
-      <c r="J25" s="26">
+      <c r="I25">
+        <v>0</v>
+      </c>
+      <c r="J25">
         <v>168750</v>
       </c>
-      <c r="K25" s="26">
-        <v>0</v>
-      </c>
-      <c r="L25" s="26">
-        <v>0</v>
-      </c>
-      <c r="M25" s="26">
-        <v>0</v>
-      </c>
-      <c r="N25" s="26">
-        <v>0</v>
-      </c>
-      <c r="O25" s="26">
-        <v>-1317.15</v>
-      </c>
-      <c r="P25" s="26">
-        <v>0.45609899999999998</v>
-      </c>
-      <c r="Q25" s="26">
+      <c r="K25">
+        <v>0</v>
+      </c>
+      <c r="L25">
+        <v>0</v>
+      </c>
+      <c r="M25">
+        <v>0</v>
+      </c>
+      <c r="N25">
+        <v>0</v>
+      </c>
+      <c r="O25">
+        <v>-32004.820936638986</v>
+      </c>
+      <c r="P25">
+        <v>0.45609893014084801</v>
+      </c>
+      <c r="Q25">
         <v>0.5</v>
       </c>
-      <c r="R25" s="26">
-        <v>0.49926199999999998</v>
-      </c>
-      <c r="S25" s="26">
+      <c r="R25">
+        <v>0.49926209763026103</v>
+      </c>
+      <c r="S25">
         <v>1</v>
       </c>
-      <c r="T25" s="26">
-        <v>-1057314</v>
-      </c>
-      <c r="U25" s="26">
-        <v>-1317.15</v>
-      </c>
-      <c r="V25" s="26">
-        <v>0.26045200000000002</v>
-      </c>
-      <c r="W25" s="26">
+      <c r="T25">
+        <v>-1057314.4805999</v>
+      </c>
+      <c r="U25">
+        <v>-32004.820936639098</v>
+      </c>
+      <c r="V25">
+        <v>0.26045217100000001</v>
+      </c>
+      <c r="W25">
         <v>0.20463000000000001</v>
       </c>
       <c r="X25" s="28">
         <f t="shared" si="0"/>
-        <v>-1057314</v>
+        <v>-1057314.4805999</v>
       </c>
       <c r="Y25" s="28">
         <f t="shared" si="1"/>
@@ -5396,7 +5385,7 @@
       </c>
       <c r="Z25" s="28">
         <f t="shared" si="2"/>
-        <v>-1317.15</v>
+        <v>-32004.820936639098</v>
       </c>
       <c r="AA25" s="28">
         <f t="shared" si="3"/>
@@ -5404,15 +5393,15 @@
       </c>
       <c r="AB25" s="30">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>2.0954757928848267E-9</v>
       </c>
       <c r="AC25" s="30">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1.127773430198431E-10</v>
       </c>
       <c r="AD25" s="30">
         <f t="shared" si="6"/>
-        <v>9.3223206931725144E-11</v>
+        <v>2.0991137716919184E-9</v>
       </c>
       <c r="AE25" s="30">
         <f>IF('Day1'!A25&lt;KPI!$B$15,1,0)</f>
@@ -5424,31 +5413,27 @@
       </c>
       <c r="AG25" s="30">
         <f t="shared" si="7"/>
-        <v>-500701</v>
+        <v>-1057314.4805999</v>
       </c>
       <c r="AH25" s="30">
         <f t="shared" si="8"/>
-        <v>-1317.15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:34" x14ac:dyDescent="0.3">
       <c r="S26" s="5">
         <f>SUM(T2:T25)</f>
-        <v>-1892035.4000000004</v>
+        <v>-1892035.3767864183</v>
       </c>
       <c r="T26" s="5">
         <f>SUM(U2:U25)</f>
-        <v>-2009808.65</v>
+        <v>-13811243.675793158</v>
       </c>
       <c r="W26" s="5"/>
       <c r="X26" s="5"/>
       <c r="Y26" s="5"/>
       <c r="Z26" s="5"/>
-      <c r="AA26" s="34"/>
-      <c r="AE26" s="31"/>
-      <c r="AF26" s="31"/>
-      <c r="AG26" s="31"/>
-      <c r="AH26" s="31"/>
+      <c r="AA26" s="5"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="Z2:Z25">
@@ -5464,7 +5449,7 @@
   <dimension ref="A1:B25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A9" sqref="A9:B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5479,7 +5464,7 @@
       </c>
       <c r="B1">
         <f>(B10+B12)/(B9+B11)</f>
-        <v>0.92790195989761171</v>
+        <v>0.92790212756060408</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -5491,9 +5476,9 @@
       <c r="A3" t="s">
         <v>13</v>
       </c>
-      <c r="B3">
-        <f>1/(KPI!B11+KPI!B12)</f>
-        <v>3.7596900276936513E-8</v>
+      <c r="B3" cm="1">
+        <f t="array" ref="B3">(SUM(-'Day1'!AG2:AG25)+SUM('Day1'!AH2:AH25))/(KPI!B11+KPI!B12)</f>
+        <v>0.56606396744346699</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -5516,63 +5501,54 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>73</v>
-      </c>
-      <c r="B8" cm="1">
-        <f t="array" ref="B8">SUM(ABS('Day1'!AB2:AB25))</f>
-        <v>6.6000000001877197</v>
-      </c>
-    </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B9">
         <f>SUM('Day1'!C2:D25)</f>
-        <v>11682771.1</v>
+        <v>11682768.75</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B10" cm="1">
         <f t="array" ref="B10">SUM(-'Day1'!E2:E25)</f>
-        <v>11705466</v>
+        <v>11705468.14997106</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B11" cm="1">
         <f t="array" ref="B11">SUM(-'Day1'!X2:X25)</f>
-        <v>14244986.4</v>
+        <v>14244986.308052372</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B12">
         <f>SUM('Day1'!Y2:Y25)</f>
-        <v>12352951</v>
+        <v>12352950.93126595</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B13" cm="1">
         <f t="array" ref="B13">SUM(-'Day1'!Z2:Z25)</f>
-        <v>2009808.65</v>
+        <v>13811243.675793158</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B14">
         <f>SUM('Day1'!AA2:AA25)</f>
@@ -5581,7 +5557,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B15">
         <f>MEDIAN('Day1'!A2:A25)</f>
@@ -5619,9 +5595,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5769,26 +5748,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1E670AA9-F151-4010-B386-EB5DE9535379}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DBD18A33-B229-4418-B69D-310A1D0DAB44}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="32e2fcb7-33f7-4889-999c-af43743a67a2"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -5812,9 +5780,17 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DBD18A33-B229-4418-B69D-310A1D0DAB44}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1E670AA9-F151-4010-B386-EB5DE9535379}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="32e2fcb7-33f7-4889-999c-af43743a67a2"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>